<commit_message>
review de patterns acabada e atualizei o backlog
</commit_message>
<xml_diff>
--- a/scrum/Phase1/Sprint1/Sprint_backlog.xlsx
+++ b/scrum/Phase1/Sprint1/Sprint_backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tduar\IdeaProjects\SE2122_57464_58763_57677_58125_63764\scrum\Phase1\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nova pasta\SE2122_57464_58763_57677_58125_63764\scrum\Phase1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D4B316-C7E8-44B1-B2F6-D0C61234879E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E4FDD7-93CE-4501-BF9B-487C74FD8BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
+    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -70,17 +70,6 @@
     <t>Metrics</t>
   </si>
   <si>
-    <t xml:space="preserve">Member 5: finished code smells.
-Member 1: finished code smells.
-Member 2: finished code smells.
-Member 3: finished code smells </t>
-  </si>
-  <si>
-    <t>Member 2: finished pattern detection
-Member 5: finished pattern detection
-Member 3: finished pattern detection</t>
-  </si>
-  <si>
     <t>Member 2: making diagrams
 Member 5: making diagrams
 Member 3: making diagrams
@@ -100,22 +89,39 @@
     <t>Member 2: Reviewing</t>
   </si>
   <si>
-    <t>Member 1: finished Reviews.
-Member 5: finished Reviews.</t>
+    <t xml:space="preserve">Member 5: finished doing the metrics
+Member 1: finished doing the metrics
+</t>
   </si>
   <si>
-    <t>Member 5: finished Reviews.</t>
+    <t>Member 2: Doing the metrics
+Member 3: finished doing the metrics</t>
   </si>
   <si>
-    <t>Member 1: Reviewing</t>
+    <t>Member 2: Reviewing
+Member 3: Reviewing</t>
   </si>
   <si>
-    <t>Member 2: Doing the metrics</t>
+    <t>Member 1: finished Reviews.
+Member 5: finished Reviews.
+Member 2: finished Reviews.</t>
   </si>
   <si>
-    <t>Member 5: finished doing the metrics
-Member 1: finished doing the metrics
-Member 3: finished doing the metrics</t>
+    <t>Member 5: finished code smells.
+Member 1: finished code smells.
+Member 2: finished code smells.
+Member 3: finished code smells 
+Member 4: finished code smells</t>
+  </si>
+  <si>
+    <t>Member 2: finished pattern detection
+Member 5: finished pattern detection
+Member 3: finished pattern detection
+Member 1: finished pattern detection</t>
+  </si>
+  <si>
+    <t>Member 5: finished Reviews.
+Member 1: finished Reviews.</t>
   </si>
 </sst>
 </file>
@@ -238,14 +244,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,11 +262,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -268,14 +280,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -595,34 +601,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0899AEA-CFD5-4FE7-96CD-5876EC28C07C}">
   <dimension ref="A1:AL161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:L18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="46.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:38" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -647,32 +653,32 @@
       <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
     </row>
-    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="6" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="6" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="6" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="6" t="s">
-        <v>15</v>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="7" t="s">
+        <v>13</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -696,29 +702,27 @@
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="8" t="s">
-        <v>13</v>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3" t="s">
+        <v>17</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="8" t="s">
-        <v>16</v>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="12" t="s">
+        <v>19</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="4" t="s">
-        <v>17</v>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -745,19 +749,19 @@
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -784,19 +788,19 @@
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
@@ -823,19 +827,19 @@
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
     </row>
-    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
@@ -862,25 +866,25 @@
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
     </row>
-    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="8" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="4" t="s">
-        <v>12</v>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
@@ -907,19 +911,19 @@
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
@@ -946,19 +950,19 @@
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
@@ -985,19 +989,19 @@
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
     </row>
-    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -1024,29 +1028,29 @@
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="8" t="s">
-        <v>13</v>
+      <c r="D11" s="3" t="s">
+        <v>11</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="4" t="s">
-        <v>19</v>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="4" t="s">
-        <v>11</v>
+      <c r="J11" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="5" t="s">
-        <v>18</v>
+      <c r="M11" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -1073,7 +1077,7 @@
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1112,7 +1116,7 @@
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1151,7 +1155,7 @@
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
     </row>
-    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1190,24 +1194,24 @@
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="8" t="s">
-        <v>14</v>
+      <c r="D15" s="3" t="s">
+        <v>12</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="4" t="s">
-        <v>20</v>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="4" t="s">
-        <v>21</v>
+      <c r="J15" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -1237,7 +1241,7 @@
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1276,7 +1280,7 @@
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1315,7 +1319,7 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
     </row>
-    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1354,7 +1358,7 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1381,7 +1385,7 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1408,7 +1412,7 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -1435,7 +1439,7 @@
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -1462,7 +1466,7 @@
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -1489,7 +1493,7 @@
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -1516,7 +1520,7 @@
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -1543,7 +1547,7 @@
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -1570,7 +1574,7 @@
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -1597,7 +1601,7 @@
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -1624,7 +1628,7 @@
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
@@ -1651,7 +1655,7 @@
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -1678,7 +1682,7 @@
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -1705,7 +1709,7 @@
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -1732,7 +1736,7 @@
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
     </row>
-    <row r="33" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -1759,7 +1763,7 @@
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
     </row>
-    <row r="34" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -1786,7 +1790,7 @@
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
     </row>
-    <row r="35" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -1813,7 +1817,7 @@
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
     </row>
-    <row r="36" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
@@ -1840,7 +1844,7 @@
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
     </row>
-    <row r="37" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="37" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
@@ -1867,7 +1871,7 @@
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
     </row>
-    <row r="38" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
@@ -1894,7 +1898,7 @@
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
     </row>
-    <row r="39" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
@@ -1921,7 +1925,7 @@
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
     </row>
-    <row r="40" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="40" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
@@ -1948,7 +1952,7 @@
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
     </row>
-    <row r="41" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="41" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
@@ -1975,7 +1979,7 @@
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
     </row>
-    <row r="42" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="42" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
@@ -2002,7 +2006,7 @@
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
     </row>
-    <row r="43" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="43" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
@@ -2029,7 +2033,7 @@
       <c r="AJ43" s="1"/>
       <c r="AK43" s="1"/>
     </row>
-    <row r="44" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="44" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
@@ -2056,7 +2060,7 @@
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
     </row>
-    <row r="45" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="45" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
@@ -2083,7 +2087,7 @@
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
     </row>
-    <row r="46" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="46" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
@@ -2110,7 +2114,7 @@
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
     </row>
-    <row r="47" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="47" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
@@ -2137,7 +2141,7 @@
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
     </row>
-    <row r="48" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="48" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
@@ -2164,7 +2168,7 @@
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
     </row>
-    <row r="49" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="49" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
@@ -2191,7 +2195,7 @@
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
     </row>
-    <row r="50" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="50" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
@@ -2218,7 +2222,7 @@
       <c r="AJ50" s="1"/>
       <c r="AK50" s="1"/>
     </row>
-    <row r="51" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="51" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
@@ -2245,7 +2249,7 @@
       <c r="AJ51" s="1"/>
       <c r="AK51" s="1"/>
     </row>
-    <row r="52" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="52" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
@@ -2272,7 +2276,7 @@
       <c r="AJ52" s="1"/>
       <c r="AK52" s="1"/>
     </row>
-    <row r="53" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="53" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
@@ -2299,7 +2303,7 @@
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
     </row>
-    <row r="54" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="54" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
@@ -2326,7 +2330,7 @@
       <c r="AJ54" s="1"/>
       <c r="AK54" s="1"/>
     </row>
-    <row r="55" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="55" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
@@ -2353,7 +2357,7 @@
       <c r="AJ55" s="1"/>
       <c r="AK55" s="1"/>
     </row>
-    <row r="56" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="56" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
@@ -2380,7 +2384,7 @@
       <c r="AJ56" s="1"/>
       <c r="AK56" s="1"/>
     </row>
-    <row r="57" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="57" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
@@ -2407,7 +2411,7 @@
       <c r="AJ57" s="1"/>
       <c r="AK57" s="1"/>
     </row>
-    <row r="58" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="58" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
@@ -2434,7 +2438,7 @@
       <c r="AJ58" s="1"/>
       <c r="AK58" s="1"/>
     </row>
-    <row r="59" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="59" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
@@ -2461,7 +2465,7 @@
       <c r="AJ59" s="1"/>
       <c r="AK59" s="1"/>
     </row>
-    <row r="60" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="60" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
@@ -2488,7 +2492,7 @@
       <c r="AJ60" s="1"/>
       <c r="AK60" s="1"/>
     </row>
-    <row r="61" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="61" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
@@ -2515,7 +2519,7 @@
       <c r="AJ61" s="1"/>
       <c r="AK61" s="1"/>
     </row>
-    <row r="62" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="62" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
@@ -2542,7 +2546,7 @@
       <c r="AJ62" s="1"/>
       <c r="AK62" s="1"/>
     </row>
-    <row r="63" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="63" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
@@ -2569,7 +2573,7 @@
       <c r="AJ63" s="1"/>
       <c r="AK63" s="1"/>
     </row>
-    <row r="64" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="64" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
@@ -2596,7 +2600,7 @@
       <c r="AJ64" s="1"/>
       <c r="AK64" s="1"/>
     </row>
-    <row r="65" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="65" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
@@ -2623,7 +2627,7 @@
       <c r="AJ65" s="1"/>
       <c r="AK65" s="1"/>
     </row>
-    <row r="66" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="66" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
       <c r="O66" s="1"/>
@@ -2650,7 +2654,7 @@
       <c r="AJ66" s="1"/>
       <c r="AK66" s="1"/>
     </row>
-    <row r="67" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="67" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
@@ -2677,7 +2681,7 @@
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
     </row>
-    <row r="68" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="68" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
@@ -2704,7 +2708,7 @@
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
     </row>
-    <row r="69" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="69" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
@@ -2731,7 +2735,7 @@
       <c r="AJ69" s="1"/>
       <c r="AK69" s="1"/>
     </row>
-    <row r="70" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="70" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
@@ -2758,7 +2762,7 @@
       <c r="AJ70" s="1"/>
       <c r="AK70" s="1"/>
     </row>
-    <row r="71" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="71" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
@@ -2785,7 +2789,7 @@
       <c r="AJ71" s="1"/>
       <c r="AK71" s="1"/>
     </row>
-    <row r="72" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="72" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
@@ -2812,7 +2816,7 @@
       <c r="AJ72" s="1"/>
       <c r="AK72" s="1"/>
     </row>
-    <row r="73" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="73" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
@@ -2839,7 +2843,7 @@
       <c r="AJ73" s="1"/>
       <c r="AK73" s="1"/>
     </row>
-    <row r="74" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="74" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
@@ -2866,7 +2870,7 @@
       <c r="AJ74" s="1"/>
       <c r="AK74" s="1"/>
     </row>
-    <row r="75" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="75" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
@@ -2893,7 +2897,7 @@
       <c r="AJ75" s="1"/>
       <c r="AK75" s="1"/>
     </row>
-    <row r="76" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="76" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
@@ -2920,7 +2924,7 @@
       <c r="AJ76" s="1"/>
       <c r="AK76" s="1"/>
     </row>
-    <row r="77" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="77" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
@@ -2947,7 +2951,7 @@
       <c r="AJ77" s="1"/>
       <c r="AK77" s="1"/>
     </row>
-    <row r="78" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="78" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
@@ -2974,7 +2978,7 @@
       <c r="AJ78" s="1"/>
       <c r="AK78" s="1"/>
     </row>
-    <row r="79" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="79" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
@@ -3001,7 +3005,7 @@
       <c r="AJ79" s="1"/>
       <c r="AK79" s="1"/>
     </row>
-    <row r="80" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="80" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
@@ -3028,7 +3032,7 @@
       <c r="AJ80" s="1"/>
       <c r="AK80" s="1"/>
     </row>
-    <row r="81" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="81" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
@@ -3055,7 +3059,7 @@
       <c r="AJ81" s="1"/>
       <c r="AK81" s="1"/>
     </row>
-    <row r="82" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="82" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
@@ -3082,7 +3086,7 @@
       <c r="AJ82" s="1"/>
       <c r="AK82" s="1"/>
     </row>
-    <row r="83" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="83" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
@@ -3109,7 +3113,7 @@
       <c r="AJ83" s="1"/>
       <c r="AK83" s="1"/>
     </row>
-    <row r="84" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="84" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
       <c r="O84" s="1"/>
@@ -3136,7 +3140,7 @@
       <c r="AJ84" s="1"/>
       <c r="AK84" s="1"/>
     </row>
-    <row r="85" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="85" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
       <c r="O85" s="1"/>
@@ -3163,7 +3167,7 @@
       <c r="AJ85" s="1"/>
       <c r="AK85" s="1"/>
     </row>
-    <row r="86" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="86" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
       <c r="O86" s="1"/>
@@ -3190,7 +3194,7 @@
       <c r="AJ86" s="1"/>
       <c r="AK86" s="1"/>
     </row>
-    <row r="87" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="87" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
       <c r="O87" s="1"/>
@@ -3217,7 +3221,7 @@
       <c r="AJ87" s="1"/>
       <c r="AK87" s="1"/>
     </row>
-    <row r="88" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="88" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
       <c r="O88" s="1"/>
@@ -3244,7 +3248,7 @@
       <c r="AJ88" s="1"/>
       <c r="AK88" s="1"/>
     </row>
-    <row r="89" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="89" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1"/>
@@ -3271,7 +3275,7 @@
       <c r="AJ89" s="1"/>
       <c r="AK89" s="1"/>
     </row>
-    <row r="90" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="90" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1"/>
@@ -3298,7 +3302,7 @@
       <c r="AJ90" s="1"/>
       <c r="AK90" s="1"/>
     </row>
-    <row r="91" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="91" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
       <c r="O91" s="1"/>
@@ -3325,7 +3329,7 @@
       <c r="AJ91" s="1"/>
       <c r="AK91" s="1"/>
     </row>
-    <row r="92" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="92" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
       <c r="O92" s="1"/>
@@ -3352,7 +3356,7 @@
       <c r="AJ92" s="1"/>
       <c r="AK92" s="1"/>
     </row>
-    <row r="93" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="93" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
       <c r="O93" s="1"/>
@@ -3379,7 +3383,7 @@
       <c r="AJ93" s="1"/>
       <c r="AK93" s="1"/>
     </row>
-    <row r="94" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="94" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
       <c r="O94" s="1"/>
@@ -3406,7 +3410,7 @@
       <c r="AJ94" s="1"/>
       <c r="AK94" s="1"/>
     </row>
-    <row r="95" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="95" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M95" s="1"/>
       <c r="N95" s="1"/>
       <c r="O95" s="1"/>
@@ -3433,7 +3437,7 @@
       <c r="AJ95" s="1"/>
       <c r="AK95" s="1"/>
     </row>
-    <row r="96" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="96" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
       <c r="O96" s="1"/>
@@ -3460,7 +3464,7 @@
       <c r="AJ96" s="1"/>
       <c r="AK96" s="1"/>
     </row>
-    <row r="97" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="97" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
       <c r="O97" s="1"/>
@@ -3487,7 +3491,7 @@
       <c r="AJ97" s="1"/>
       <c r="AK97" s="1"/>
     </row>
-    <row r="98" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="98" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
       <c r="O98" s="1"/>
@@ -3514,7 +3518,7 @@
       <c r="AJ98" s="1"/>
       <c r="AK98" s="1"/>
     </row>
-    <row r="99" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="99" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
       <c r="O99" s="1"/>
@@ -3541,7 +3545,7 @@
       <c r="AJ99" s="1"/>
       <c r="AK99" s="1"/>
     </row>
-    <row r="100" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="100" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
       <c r="O100" s="1"/>
@@ -3568,7 +3572,7 @@
       <c r="AJ100" s="1"/>
       <c r="AK100" s="1"/>
     </row>
-    <row r="101" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="101" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
       <c r="O101" s="1"/>
@@ -3595,7 +3599,7 @@
       <c r="AJ101" s="1"/>
       <c r="AK101" s="1"/>
     </row>
-    <row r="102" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="102" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
       <c r="O102" s="1"/>
@@ -3622,7 +3626,7 @@
       <c r="AJ102" s="1"/>
       <c r="AK102" s="1"/>
     </row>
-    <row r="103" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="103" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
       <c r="O103" s="1"/>
@@ -3649,7 +3653,7 @@
       <c r="AJ103" s="1"/>
       <c r="AK103" s="1"/>
     </row>
-    <row r="104" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="104" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
       <c r="O104" s="1"/>
@@ -3676,7 +3680,7 @@
       <c r="AJ104" s="1"/>
       <c r="AK104" s="1"/>
     </row>
-    <row r="105" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="105" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M105" s="1"/>
       <c r="N105" s="1"/>
       <c r="O105" s="1"/>
@@ -3703,7 +3707,7 @@
       <c r="AJ105" s="1"/>
       <c r="AK105" s="1"/>
     </row>
-    <row r="106" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="106" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
       <c r="O106" s="1"/>
@@ -3730,7 +3734,7 @@
       <c r="AJ106" s="1"/>
       <c r="AK106" s="1"/>
     </row>
-    <row r="107" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="107" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M107" s="1"/>
       <c r="N107" s="1"/>
       <c r="O107" s="1"/>
@@ -3757,7 +3761,7 @@
       <c r="AJ107" s="1"/>
       <c r="AK107" s="1"/>
     </row>
-    <row r="108" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="108" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M108" s="1"/>
       <c r="N108" s="1"/>
       <c r="O108" s="1"/>
@@ -3784,7 +3788,7 @@
       <c r="AJ108" s="1"/>
       <c r="AK108" s="1"/>
     </row>
-    <row r="109" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="109" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M109" s="1"/>
       <c r="N109" s="1"/>
       <c r="O109" s="1"/>
@@ -3811,7 +3815,7 @@
       <c r="AJ109" s="1"/>
       <c r="AK109" s="1"/>
     </row>
-    <row r="110" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="110" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M110" s="1"/>
       <c r="N110" s="1"/>
       <c r="O110" s="1"/>
@@ -3838,7 +3842,7 @@
       <c r="AJ110" s="1"/>
       <c r="AK110" s="1"/>
     </row>
-    <row r="111" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="111" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M111" s="1"/>
       <c r="N111" s="1"/>
       <c r="O111" s="1"/>
@@ -3865,7 +3869,7 @@
       <c r="AJ111" s="1"/>
       <c r="AK111" s="1"/>
     </row>
-    <row r="112" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="112" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M112" s="1"/>
       <c r="N112" s="1"/>
       <c r="O112" s="1"/>
@@ -3892,7 +3896,7 @@
       <c r="AJ112" s="1"/>
       <c r="AK112" s="1"/>
     </row>
-    <row r="113" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="113" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M113" s="1"/>
       <c r="N113" s="1"/>
       <c r="O113" s="1"/>
@@ -3919,7 +3923,7 @@
       <c r="AJ113" s="1"/>
       <c r="AK113" s="1"/>
     </row>
-    <row r="114" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="114" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M114" s="1"/>
       <c r="N114" s="1"/>
       <c r="O114" s="1"/>
@@ -3946,7 +3950,7 @@
       <c r="AJ114" s="1"/>
       <c r="AK114" s="1"/>
     </row>
-    <row r="115" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="115" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M115" s="1"/>
       <c r="N115" s="1"/>
       <c r="O115" s="1"/>
@@ -3973,7 +3977,7 @@
       <c r="AJ115" s="1"/>
       <c r="AK115" s="1"/>
     </row>
-    <row r="116" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="116" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M116" s="1"/>
       <c r="N116" s="1"/>
       <c r="O116" s="1"/>
@@ -4000,7 +4004,7 @@
       <c r="AJ116" s="1"/>
       <c r="AK116" s="1"/>
     </row>
-    <row r="117" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="117" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M117" s="1"/>
       <c r="N117" s="1"/>
       <c r="O117" s="1"/>
@@ -4027,7 +4031,7 @@
       <c r="AJ117" s="1"/>
       <c r="AK117" s="1"/>
     </row>
-    <row r="118" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="118" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M118" s="1"/>
       <c r="N118" s="1"/>
       <c r="O118" s="1"/>
@@ -4054,7 +4058,7 @@
       <c r="AJ118" s="1"/>
       <c r="AK118" s="1"/>
     </row>
-    <row r="119" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="119" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M119" s="1"/>
       <c r="N119" s="1"/>
       <c r="O119" s="1"/>
@@ -4081,7 +4085,7 @@
       <c r="AJ119" s="1"/>
       <c r="AK119" s="1"/>
     </row>
-    <row r="120" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="120" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M120" s="1"/>
       <c r="N120" s="1"/>
       <c r="O120" s="1"/>
@@ -4108,7 +4112,7 @@
       <c r="AJ120" s="1"/>
       <c r="AK120" s="1"/>
     </row>
-    <row r="121" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="121" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M121" s="1"/>
       <c r="N121" s="1"/>
       <c r="O121" s="1"/>
@@ -4135,7 +4139,7 @@
       <c r="AJ121" s="1"/>
       <c r="AK121" s="1"/>
     </row>
-    <row r="122" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="122" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M122" s="1"/>
       <c r="N122" s="1"/>
       <c r="O122" s="1"/>
@@ -4162,7 +4166,7 @@
       <c r="AJ122" s="1"/>
       <c r="AK122" s="1"/>
     </row>
-    <row r="123" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="123" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M123" s="1"/>
       <c r="N123" s="1"/>
       <c r="O123" s="1"/>
@@ -4189,7 +4193,7 @@
       <c r="AJ123" s="1"/>
       <c r="AK123" s="1"/>
     </row>
-    <row r="124" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="124" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M124" s="1"/>
       <c r="N124" s="1"/>
       <c r="O124" s="1"/>
@@ -4216,7 +4220,7 @@
       <c r="AJ124" s="1"/>
       <c r="AK124" s="1"/>
     </row>
-    <row r="125" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="125" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M125" s="1"/>
       <c r="N125" s="1"/>
       <c r="O125" s="1"/>
@@ -4243,7 +4247,7 @@
       <c r="AJ125" s="1"/>
       <c r="AK125" s="1"/>
     </row>
-    <row r="126" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="126" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M126" s="1"/>
       <c r="N126" s="1"/>
       <c r="O126" s="1"/>
@@ -4270,7 +4274,7 @@
       <c r="AJ126" s="1"/>
       <c r="AK126" s="1"/>
     </row>
-    <row r="127" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="127" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
       <c r="O127" s="1"/>
@@ -4297,7 +4301,7 @@
       <c r="AJ127" s="1"/>
       <c r="AK127" s="1"/>
     </row>
-    <row r="128" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="128" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M128" s="1"/>
       <c r="N128" s="1"/>
       <c r="O128" s="1"/>
@@ -4324,7 +4328,7 @@
       <c r="AJ128" s="1"/>
       <c r="AK128" s="1"/>
     </row>
-    <row r="129" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="129" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M129" s="1"/>
       <c r="N129" s="1"/>
       <c r="O129" s="1"/>
@@ -4351,7 +4355,7 @@
       <c r="AJ129" s="1"/>
       <c r="AK129" s="1"/>
     </row>
-    <row r="130" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="130" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M130" s="1"/>
       <c r="N130" s="1"/>
       <c r="O130" s="1"/>
@@ -4378,7 +4382,7 @@
       <c r="AJ130" s="1"/>
       <c r="AK130" s="1"/>
     </row>
-    <row r="131" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="131" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M131" s="1"/>
       <c r="N131" s="1"/>
       <c r="O131" s="1"/>
@@ -4405,7 +4409,7 @@
       <c r="AJ131" s="1"/>
       <c r="AK131" s="1"/>
     </row>
-    <row r="132" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="132" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M132" s="1"/>
       <c r="N132" s="1"/>
       <c r="O132" s="1"/>
@@ -4432,7 +4436,7 @@
       <c r="AJ132" s="1"/>
       <c r="AK132" s="1"/>
     </row>
-    <row r="133" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="133" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M133" s="1"/>
       <c r="N133" s="1"/>
       <c r="O133" s="1"/>
@@ -4459,7 +4463,7 @@
       <c r="AJ133" s="1"/>
       <c r="AK133" s="1"/>
     </row>
-    <row r="134" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="134" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M134" s="1"/>
       <c r="N134" s="1"/>
       <c r="O134" s="1"/>
@@ -4486,7 +4490,7 @@
       <c r="AJ134" s="1"/>
       <c r="AK134" s="1"/>
     </row>
-    <row r="135" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="135" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M135" s="1"/>
       <c r="N135" s="1"/>
       <c r="O135" s="1"/>
@@ -4513,7 +4517,7 @@
       <c r="AJ135" s="1"/>
       <c r="AK135" s="1"/>
     </row>
-    <row r="136" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="136" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M136" s="1"/>
       <c r="N136" s="1"/>
       <c r="O136" s="1"/>
@@ -4540,7 +4544,7 @@
       <c r="AJ136" s="1"/>
       <c r="AK136" s="1"/>
     </row>
-    <row r="137" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="137" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M137" s="1"/>
       <c r="N137" s="1"/>
       <c r="O137" s="1"/>
@@ -4567,7 +4571,7 @@
       <c r="AJ137" s="1"/>
       <c r="AK137" s="1"/>
     </row>
-    <row r="138" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="138" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M138" s="1"/>
       <c r="N138" s="1"/>
       <c r="O138" s="1"/>
@@ -4594,7 +4598,7 @@
       <c r="AJ138" s="1"/>
       <c r="AK138" s="1"/>
     </row>
-    <row r="139" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="139" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M139" s="1"/>
       <c r="N139" s="1"/>
       <c r="O139" s="1"/>
@@ -4621,7 +4625,7 @@
       <c r="AJ139" s="1"/>
       <c r="AK139" s="1"/>
     </row>
-    <row r="140" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="140" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M140" s="1"/>
       <c r="N140" s="1"/>
       <c r="O140" s="1"/>
@@ -4648,7 +4652,7 @@
       <c r="AJ140" s="1"/>
       <c r="AK140" s="1"/>
     </row>
-    <row r="141" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="141" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M141" s="1"/>
       <c r="N141" s="1"/>
       <c r="O141" s="1"/>
@@ -4675,7 +4679,7 @@
       <c r="AJ141" s="1"/>
       <c r="AK141" s="1"/>
     </row>
-    <row r="142" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="142" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M142" s="1"/>
       <c r="N142" s="1"/>
       <c r="O142" s="1"/>
@@ -4702,7 +4706,7 @@
       <c r="AJ142" s="1"/>
       <c r="AK142" s="1"/>
     </row>
-    <row r="143" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="143" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M143" s="1"/>
       <c r="N143" s="1"/>
       <c r="O143" s="1"/>
@@ -4729,7 +4733,7 @@
       <c r="AJ143" s="1"/>
       <c r="AK143" s="1"/>
     </row>
-    <row r="144" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="144" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M144" s="1"/>
       <c r="N144" s="1"/>
       <c r="O144" s="1"/>
@@ -4756,7 +4760,7 @@
       <c r="AJ144" s="1"/>
       <c r="AK144" s="1"/>
     </row>
-    <row r="145" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="145" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M145" s="1"/>
       <c r="N145" s="1"/>
       <c r="O145" s="1"/>
@@ -4783,7 +4787,7 @@
       <c r="AJ145" s="1"/>
       <c r="AK145" s="1"/>
     </row>
-    <row r="146" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="146" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M146" s="1"/>
       <c r="N146" s="1"/>
       <c r="O146" s="1"/>
@@ -4810,7 +4814,7 @@
       <c r="AJ146" s="1"/>
       <c r="AK146" s="1"/>
     </row>
-    <row r="147" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="147" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M147" s="1"/>
       <c r="N147" s="1"/>
       <c r="O147" s="1"/>
@@ -4837,7 +4841,7 @@
       <c r="AJ147" s="1"/>
       <c r="AK147" s="1"/>
     </row>
-    <row r="148" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="148" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M148" s="1"/>
       <c r="N148" s="1"/>
       <c r="O148" s="1"/>
@@ -4864,7 +4868,7 @@
       <c r="AJ148" s="1"/>
       <c r="AK148" s="1"/>
     </row>
-    <row r="149" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="149" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M149" s="1"/>
       <c r="N149" s="1"/>
       <c r="O149" s="1"/>
@@ -4891,7 +4895,7 @@
       <c r="AJ149" s="1"/>
       <c r="AK149" s="1"/>
     </row>
-    <row r="150" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="150" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M150" s="1"/>
       <c r="N150" s="1"/>
       <c r="O150" s="1"/>
@@ -4918,7 +4922,7 @@
       <c r="AJ150" s="1"/>
       <c r="AK150" s="1"/>
     </row>
-    <row r="151" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="151" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M151" s="1"/>
       <c r="N151" s="1"/>
       <c r="O151" s="1"/>
@@ -4945,7 +4949,7 @@
       <c r="AJ151" s="1"/>
       <c r="AK151" s="1"/>
     </row>
-    <row r="152" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="152" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M152" s="1"/>
       <c r="N152" s="1"/>
       <c r="O152" s="1"/>
@@ -4972,7 +4976,7 @@
       <c r="AJ152" s="1"/>
       <c r="AK152" s="1"/>
     </row>
-    <row r="153" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="153" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M153" s="1"/>
       <c r="N153" s="1"/>
       <c r="O153" s="1"/>
@@ -4999,7 +5003,7 @@
       <c r="AJ153" s="1"/>
       <c r="AK153" s="1"/>
     </row>
-    <row r="154" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="154" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M154" s="1"/>
       <c r="N154" s="1"/>
       <c r="O154" s="1"/>
@@ -5026,7 +5030,7 @@
       <c r="AJ154" s="1"/>
       <c r="AK154" s="1"/>
     </row>
-    <row r="155" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="155" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M155" s="1"/>
       <c r="N155" s="1"/>
       <c r="O155" s="1"/>
@@ -5053,7 +5057,7 @@
       <c r="AJ155" s="1"/>
       <c r="AK155" s="1"/>
     </row>
-    <row r="156" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="156" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M156" s="1"/>
       <c r="N156" s="1"/>
       <c r="O156" s="1"/>
@@ -5080,7 +5084,7 @@
       <c r="AJ156" s="1"/>
       <c r="AK156" s="1"/>
     </row>
-    <row r="157" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="157" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M157" s="1"/>
       <c r="N157" s="1"/>
       <c r="O157" s="1"/>
@@ -5107,7 +5111,7 @@
       <c r="AJ157" s="1"/>
       <c r="AK157" s="1"/>
     </row>
-    <row r="158" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="158" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M158" s="1"/>
       <c r="N158" s="1"/>
       <c r="O158" s="1"/>
@@ -5134,7 +5138,7 @@
       <c r="AJ158" s="1"/>
       <c r="AK158" s="1"/>
     </row>
-    <row r="159" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="159" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M159" s="1"/>
       <c r="N159" s="1"/>
       <c r="O159" s="1"/>
@@ -5161,7 +5165,7 @@
       <c r="AJ159" s="1"/>
       <c r="AK159" s="1"/>
     </row>
-    <row r="160" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="160" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M160" s="1"/>
       <c r="N160" s="1"/>
       <c r="O160" s="1"/>
@@ -5188,7 +5192,7 @@
       <c r="AJ160" s="1"/>
       <c r="AK160" s="1"/>
     </row>
-    <row r="161" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="161" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M161" s="1"/>
       <c r="N161" s="1"/>
       <c r="O161" s="1"/>
@@ -5217,16 +5221,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D11:F14"/>
-    <mergeCell ref="G11:I14"/>
-    <mergeCell ref="J11:L14"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="A3:C6"/>
-    <mergeCell ref="D3:F6"/>
-    <mergeCell ref="G3:I6"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="M3:O6"/>
     <mergeCell ref="M7:O10"/>
@@ -5243,6 +5237,16 @@
     <mergeCell ref="G7:I10"/>
     <mergeCell ref="J7:L10"/>
     <mergeCell ref="A11:C14"/>
+    <mergeCell ref="D11:F14"/>
+    <mergeCell ref="G11:I14"/>
+    <mergeCell ref="J11:L14"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="A3:C6"/>
+    <mergeCell ref="D3:F6"/>
+    <mergeCell ref="G3:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5250,6 +5254,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008EA8F6205B617B4CBD762DBD6D300502" ma:contentTypeVersion="4" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="000a41c94a85e4495c2f2d3453c30ed1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="10b95d85-a823-4616-89f6-0a6587d88b0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0729d4038857d2ede91d1e28869f4e90" ns3:_="">
     <xsd:import namespace="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
@@ -5395,35 +5414,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A39B317-7C09-4361-8F9C-EC6B55EB4D12}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5445,9 +5439,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A39B317-7C09-4361-8F9C-EC6B55EB4D12}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
elem2 patterns review updated and sprint backlog update
</commit_message>
<xml_diff>
--- a/scrum/Phase1/Sprint1/Sprint_backlog.xlsx
+++ b/scrum/Phase1/Sprint1/Sprint_backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\Faculdade\3º Ano\1º Semestre\ES\jabref\scrum\Phase1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A869D7-B464-47A7-B412-B5984B86A6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347EBF5F-2059-4F35-8AB5-19F557A64951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Review</t>
   </si>
   <si>
-    <t>Member 2: Reviewing</t>
-  </si>
-  <si>
     <t>Member 2: Reviewing
 Member 3: Reviewing</t>
   </si>
@@ -111,10 +108,6 @@
 Member 1: finished pattern detection</t>
   </si>
   <si>
-    <t>Member 5: finished Reviews.
-Member 1: finished Reviews.</t>
-  </si>
-  <si>
     <t>Member 3:  doing the metrics</t>
   </si>
   <si>
@@ -126,6 +119,11 @@
 Member 1: finished doing the metrics
 Member 2: finished doing the metrics
 </t>
+  </si>
+  <si>
+    <t>Member 5: finished Reviews.
+Member 1: finished Reviews.
+Member 2: finished Reviews.</t>
   </si>
 </sst>
 </file>
@@ -248,17 +246,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -266,14 +261,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -284,8 +276,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -606,7 +604,7 @@
   <dimension ref="A1:AL161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="M15" sqref="M15:O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,23 +614,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -658,31 +656,31 @@
       <c r="AL1" s="1"/>
     </row>
     <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="7" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="7" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="7" t="s">
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -707,26 +705,26 @@
       <c r="AK2" s="1"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="3" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -754,18 +752,18 @@
       <c r="AK3" s="1"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -793,18 +791,18 @@
       <c r="AK4" s="1"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
@@ -832,18 +830,18 @@
       <c r="AK5" s="1"/>
     </row>
     <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
@@ -871,24 +869,24 @@
       <c r="AK6" s="1"/>
     </row>
     <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="6" t="s">
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
@@ -916,18 +914,18 @@
       <c r="AK7" s="1"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
@@ -955,18 +953,18 @@
       <c r="AK8" s="1"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
@@ -994,18 +992,18 @@
       <c r="AK9" s="1"/>
     </row>
     <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -1038,23 +1036,21 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="4"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="6" t="s">
-        <v>18</v>
+      <c r="J11" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="6" t="s">
-        <v>19</v>
+      <c r="M11" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -1204,23 +1200,23 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="6" t="s">
-        <v>20</v>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="6" t="s">
-        <v>22</v>
+      <c r="J15" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
-      <c r="M15" s="6" t="s">
-        <v>21</v>
+      <c r="M15" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
@@ -5227,6 +5223,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D11:F14"/>
+    <mergeCell ref="G11:I14"/>
+    <mergeCell ref="J11:L14"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="A3:C6"/>
+    <mergeCell ref="D3:F6"/>
+    <mergeCell ref="G3:I6"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="M3:O6"/>
     <mergeCell ref="M7:O10"/>
@@ -5243,16 +5249,6 @@
     <mergeCell ref="G7:I10"/>
     <mergeCell ref="J7:L10"/>
     <mergeCell ref="A11:C14"/>
-    <mergeCell ref="D11:F14"/>
-    <mergeCell ref="G11:I14"/>
-    <mergeCell ref="J11:L14"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="A3:C6"/>
-    <mergeCell ref="D3:F6"/>
-    <mergeCell ref="G3:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5260,18 +5256,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5421,14 +5417,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A7B2E4-0806-468A-9362-8AC839DA2BE7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -5440,6 +5428,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated Sprint backlog to use case done.
</commit_message>
<xml_diff>
--- a/scrum/Phase1/Sprint1/Sprint_backlog.xlsx
+++ b/scrum/Phase1/Sprint1/Sprint_backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djsil\IdeaProjects\SE2122_57464_58763_57677_58125_63764(4)\scrum\Phase1\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\SE2122_57464_58763_57677_58125_63764\scrum\Phase1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE248DDD-1732-46A1-BB8A-A0268E0A8AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93951C15-1893-4281-857E-17EC56B9FA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="84" yWindow="264" windowWidth="22956" windowHeight="12096" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -52,13 +52,6 @@
   </si>
   <si>
     <t>Detect code smells</t>
-  </si>
-  <si>
-    <t>Member 1: gui package
-Member 2: logic package
-Member 3: model package
-Member 4: preferences package
-Member 5: cli package</t>
   </si>
   <si>
     <t>Use Case Diagrams</t>
@@ -94,12 +87,6 @@
     <t>Member 4: Detect 3 code smells in preferences package and review 3 others</t>
   </si>
   <si>
-    <t>Member 2: making diagrams
-Member 5: making diagrams
-Member 3: making diagrams
-Member 1: making diagram Member 4: making diagrams</t>
-  </si>
-  <si>
     <t>Member 4: detect 3 design patterns in preferences package and review 3 others</t>
   </si>
   <si>
@@ -132,6 +119,20 @@
   <si>
     <t>Member 3: model package
 Member 4: do the MOOD metrics set, analyse the result and make a report.</t>
+  </si>
+  <si>
+    <t>Member 1: gui package
+Member 2: logic package
+Member 3: model package
+Member 4: preferences package</t>
+  </si>
+  <si>
+    <t>Member 2: making diagrams
+Member 3: making diagrams
+Member 1: making diagram Member 4: making diagrams</t>
+  </si>
+  <si>
+    <t>Member 5: finished Use case diagrams</t>
   </si>
 </sst>
 </file>
@@ -250,21 +251,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -272,14 +270,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -290,13 +285,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Cálculo" xfId="2" builtinId="22"/>
+    <cellStyle name="Correto" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -313,7 +311,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -611,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0899AEA-CFD5-4FE7-96CD-5876EC28C07C}">
   <dimension ref="A1:AL161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q16:Q17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,23 +620,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="46.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -664,31 +662,31 @@
       <c r="AL1" s="1"/>
     </row>
     <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="7" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="7" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="7" t="s">
-        <v>10</v>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="6" t="s">
+        <v>9</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -713,28 +711,28 @@
       <c r="AK2" s="1"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="12" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="6" t="s">
-        <v>13</v>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -762,18 +760,18 @@
       <c r="AK3" s="1"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -801,18 +799,18 @@
       <c r="AK4" s="1"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
@@ -840,18 +838,18 @@
       <c r="AK5" s="1"/>
     </row>
     <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
@@ -879,24 +877,26 @@
       <c r="AK6" s="1"/>
     </row>
     <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="6" t="s">
-        <v>15</v>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
+      <c r="J7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
@@ -924,18 +924,18 @@
       <c r="AK7" s="1"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
@@ -963,18 +963,18 @@
       <c r="AK8" s="1"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
@@ -1002,18 +1002,18 @@
       <c r="AK9" s="1"/>
     </row>
     <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -1042,27 +1042,27 @@
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
+      <c r="D11" s="8" t="s">
+        <v>14</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="6" t="s">
-        <v>17</v>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="6" t="s">
-        <v>18</v>
+      <c r="J11" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="6" t="s">
-        <v>19</v>
+      <c r="M11" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -1208,27 +1208,27 @@
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="3" t="s">
-        <v>23</v>
+      <c r="D15" s="8" t="s">
+        <v>21</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="6" t="s">
-        <v>20</v>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="6" t="s">
-        <v>21</v>
+      <c r="J15" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
-      <c r="M15" s="6" t="s">
-        <v>22</v>
+      <c r="M15" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
@@ -5235,6 +5235,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D11:F14"/>
+    <mergeCell ref="G11:I14"/>
+    <mergeCell ref="J11:L14"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="A3:C6"/>
+    <mergeCell ref="D3:F6"/>
+    <mergeCell ref="G3:I6"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="M3:O6"/>
     <mergeCell ref="M7:O10"/>
@@ -5251,16 +5261,6 @@
     <mergeCell ref="G7:I10"/>
     <mergeCell ref="J7:L10"/>
     <mergeCell ref="A11:C14"/>
-    <mergeCell ref="D11:F14"/>
-    <mergeCell ref="G11:I14"/>
-    <mergeCell ref="J11:L14"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="A3:C6"/>
-    <mergeCell ref="D3:F6"/>
-    <mergeCell ref="G3:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5268,18 +5268,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5429,14 +5429,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A7B2E4-0806-468A-9362-8AC839DA2BE7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -5448,6 +5440,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
use case diagrams and description done + sprint backlog update
</commit_message>
<xml_diff>
--- a/scrum/Phase1/Sprint1/Sprint_backlog.xlsx
+++ b/scrum/Phase1/Sprint1/Sprint_backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\SE2122_57464_58763_57677_58125_63764\scrum\Phase1\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\Faculdade\3º Ano\1º Semestre\ES\jabref\scrum\Phase1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93951C15-1893-4281-857E-17EC56B9FA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34798E2B-EBD0-4221-88B3-182874042B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -73,11 +73,6 @@
 Member 4: finished code smells</t>
   </si>
   <si>
-    <t>Member 2: Reviewing
-Member 3: Reviewing
-Member 4: Reviewing</t>
-  </si>
-  <si>
     <t>Member 1: finished Reviews.
 Member 5: finished Reviews.
 Member 2: finished Reviews.
@@ -90,27 +85,10 @@
     <t>Member 4: detect 3 design patterns in preferences package and review 3 others</t>
   </si>
   <si>
-    <t>Member 3:  doing the design patterns</t>
-  </si>
-  <si>
     <t>Member 2: finished pattern detection
 Member 5: finished pattern detection
 Member 3: finished pattern detection
 Member 1: finished pattern detection Member 4: finished pattern detection</t>
-  </si>
-  <si>
-    <t>Member 5: finished Reviews.
-Member 1: finished Reviews.
-Member 2: finished Reviews. Member 4: finished Reviews</t>
-  </si>
-  <si>
-    <t>Member 3:  doing the metrics Member 4:  doing the metrics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Member 5: finished doing the metrics
-Member 1: finished doing the metrics
-Member 2: finished doing the metrics Member 4: finished doing the metrics
-</t>
   </si>
   <si>
     <t>Member 5: finished Reviews.
@@ -127,12 +105,34 @@
 Member 4: preferences package</t>
   </si>
   <si>
-    <t>Member 2: making diagrams
-Member 3: making diagrams
-Member 1: making diagram Member 4: making diagrams</t>
+    <t xml:space="preserve">Member 5: finished Reviews.
+Member 1: finished Reviews.
+Member 2: finished Reviews. Member 4: finished Reviews.
+</t>
   </si>
   <si>
-    <t>Member 5: finished Use case diagrams</t>
+    <t>Member 3:  reviewing the design patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Member 5: finished doing the metrics
+Member 1: finished doing the metrics
+Member 2: finished doing the metrics Member 4: finished doing the metrics
+Member 3: finished doing the metrics
+</t>
+  </si>
+  <si>
+    <t>Member 3:  reviewing the metrics</t>
+  </si>
+  <si>
+    <t>Member 5: finished Use case diagrams
+Member 2: finished Use case diagrams</t>
+  </si>
+  <si>
+    <t>Member 2: reviewing diagrams
+Member 5: reviewing diagrams
+Member 3: making diagrams
+Member 1: making diagram
+Member 4: making diagrams</t>
   </si>
 </sst>
 </file>
@@ -255,14 +255,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -270,11 +273,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -283,12 +289,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -610,33 +610,34 @@
   <dimension ref="A1:AL161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="G7" sqref="G7:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="12" max="12" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="46.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:38" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -661,32 +662,32 @@
       <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
     </row>
-    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="6" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="6" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="6" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="6" t="s">
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -710,29 +711,27 @@
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="8" t="s">
-        <v>13</v>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="4" t="s">
-        <v>12</v>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -759,19 +758,19 @@
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -798,19 +797,19 @@
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
@@ -837,19 +836,19 @@
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
     </row>
-    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
+    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
@@ -876,24 +875,24 @@
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
     </row>
-    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="8" t="s">
-        <v>22</v>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="4" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="5" t="s">
-        <v>24</v>
+      <c r="J7" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -923,10 +922,10 @@
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -962,10 +961,10 @@
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -1001,10 +1000,10 @@
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
     </row>
-    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -1040,29 +1039,29 @@
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="8" t="s">
-        <v>14</v>
+      <c r="D11" s="3" t="s">
+        <v>13</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="4" t="s">
-        <v>15</v>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="4" t="s">
-        <v>16</v>
+      <c r="J11" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="4" t="s">
-        <v>17</v>
+      <c r="M11" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -1089,7 +1088,7 @@
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1128,7 +1127,7 @@
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1167,7 +1166,7 @@
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
     </row>
-    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1206,29 +1205,29 @@
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="4" t="s">
-        <v>19</v>
+      <c r="J15" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
-      <c r="M15" s="4" t="s">
-        <v>20</v>
+      <c r="M15" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
@@ -1255,7 +1254,7 @@
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1294,7 +1293,7 @@
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1333,7 +1332,7 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
     </row>
-    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1372,7 +1371,7 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1399,7 +1398,7 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1426,7 +1425,7 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -1453,7 +1452,7 @@
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -1480,7 +1479,7 @@
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -1507,7 +1506,7 @@
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -1534,7 +1533,7 @@
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -1561,7 +1560,7 @@
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -1588,7 +1587,7 @@
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -1615,7 +1614,7 @@
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -1642,7 +1641,7 @@
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
@@ -1669,7 +1668,7 @@
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -1696,7 +1695,7 @@
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -1723,7 +1722,7 @@
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -1750,7 +1749,7 @@
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
     </row>
-    <row r="33" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -1777,7 +1776,7 @@
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
     </row>
-    <row r="34" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -1804,7 +1803,7 @@
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
     </row>
-    <row r="35" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -1831,7 +1830,7 @@
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
     </row>
-    <row r="36" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
@@ -1858,7 +1857,7 @@
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
     </row>
-    <row r="37" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="37" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
@@ -1885,7 +1884,7 @@
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
     </row>
-    <row r="38" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
@@ -1912,7 +1911,7 @@
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
     </row>
-    <row r="39" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
@@ -1939,7 +1938,7 @@
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
     </row>
-    <row r="40" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="40" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
@@ -1966,7 +1965,7 @@
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
     </row>
-    <row r="41" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="41" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
@@ -1993,7 +1992,7 @@
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
     </row>
-    <row r="42" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="42" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
@@ -2020,7 +2019,7 @@
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
     </row>
-    <row r="43" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="43" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
@@ -2047,7 +2046,7 @@
       <c r="AJ43" s="1"/>
       <c r="AK43" s="1"/>
     </row>
-    <row r="44" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="44" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
@@ -2074,7 +2073,7 @@
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
     </row>
-    <row r="45" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="45" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
@@ -2101,7 +2100,7 @@
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
     </row>
-    <row r="46" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="46" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
@@ -2128,7 +2127,7 @@
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
     </row>
-    <row r="47" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="47" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
@@ -2155,7 +2154,7 @@
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
     </row>
-    <row r="48" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="48" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
@@ -2182,7 +2181,7 @@
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
     </row>
-    <row r="49" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="49" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
@@ -2209,7 +2208,7 @@
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
     </row>
-    <row r="50" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="50" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
@@ -2236,7 +2235,7 @@
       <c r="AJ50" s="1"/>
       <c r="AK50" s="1"/>
     </row>
-    <row r="51" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="51" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
@@ -2263,7 +2262,7 @@
       <c r="AJ51" s="1"/>
       <c r="AK51" s="1"/>
     </row>
-    <row r="52" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="52" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
@@ -2290,7 +2289,7 @@
       <c r="AJ52" s="1"/>
       <c r="AK52" s="1"/>
     </row>
-    <row r="53" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="53" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
@@ -2317,7 +2316,7 @@
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
     </row>
-    <row r="54" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="54" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
@@ -2344,7 +2343,7 @@
       <c r="AJ54" s="1"/>
       <c r="AK54" s="1"/>
     </row>
-    <row r="55" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="55" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
@@ -2371,7 +2370,7 @@
       <c r="AJ55" s="1"/>
       <c r="AK55" s="1"/>
     </row>
-    <row r="56" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="56" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
@@ -2398,7 +2397,7 @@
       <c r="AJ56" s="1"/>
       <c r="AK56" s="1"/>
     </row>
-    <row r="57" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="57" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
@@ -2425,7 +2424,7 @@
       <c r="AJ57" s="1"/>
       <c r="AK57" s="1"/>
     </row>
-    <row r="58" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="58" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
@@ -2452,7 +2451,7 @@
       <c r="AJ58" s="1"/>
       <c r="AK58" s="1"/>
     </row>
-    <row r="59" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="59" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
@@ -2479,7 +2478,7 @@
       <c r="AJ59" s="1"/>
       <c r="AK59" s="1"/>
     </row>
-    <row r="60" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="60" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
@@ -2506,7 +2505,7 @@
       <c r="AJ60" s="1"/>
       <c r="AK60" s="1"/>
     </row>
-    <row r="61" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="61" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
@@ -2533,7 +2532,7 @@
       <c r="AJ61" s="1"/>
       <c r="AK61" s="1"/>
     </row>
-    <row r="62" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="62" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
@@ -2560,7 +2559,7 @@
       <c r="AJ62" s="1"/>
       <c r="AK62" s="1"/>
     </row>
-    <row r="63" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="63" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
@@ -2587,7 +2586,7 @@
       <c r="AJ63" s="1"/>
       <c r="AK63" s="1"/>
     </row>
-    <row r="64" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="64" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
@@ -2614,7 +2613,7 @@
       <c r="AJ64" s="1"/>
       <c r="AK64" s="1"/>
     </row>
-    <row r="65" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="65" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
@@ -2641,7 +2640,7 @@
       <c r="AJ65" s="1"/>
       <c r="AK65" s="1"/>
     </row>
-    <row r="66" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="66" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
       <c r="O66" s="1"/>
@@ -2668,7 +2667,7 @@
       <c r="AJ66" s="1"/>
       <c r="AK66" s="1"/>
     </row>
-    <row r="67" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="67" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
@@ -2695,7 +2694,7 @@
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
     </row>
-    <row r="68" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="68" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
@@ -2722,7 +2721,7 @@
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
     </row>
-    <row r="69" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="69" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
@@ -2749,7 +2748,7 @@
       <c r="AJ69" s="1"/>
       <c r="AK69" s="1"/>
     </row>
-    <row r="70" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="70" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
@@ -2776,7 +2775,7 @@
       <c r="AJ70" s="1"/>
       <c r="AK70" s="1"/>
     </row>
-    <row r="71" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="71" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
@@ -2803,7 +2802,7 @@
       <c r="AJ71" s="1"/>
       <c r="AK71" s="1"/>
     </row>
-    <row r="72" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="72" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
@@ -2830,7 +2829,7 @@
       <c r="AJ72" s="1"/>
       <c r="AK72" s="1"/>
     </row>
-    <row r="73" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="73" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
@@ -2857,7 +2856,7 @@
       <c r="AJ73" s="1"/>
       <c r="AK73" s="1"/>
     </row>
-    <row r="74" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="74" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
@@ -2884,7 +2883,7 @@
       <c r="AJ74" s="1"/>
       <c r="AK74" s="1"/>
     </row>
-    <row r="75" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="75" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
@@ -2911,7 +2910,7 @@
       <c r="AJ75" s="1"/>
       <c r="AK75" s="1"/>
     </row>
-    <row r="76" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="76" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
@@ -2938,7 +2937,7 @@
       <c r="AJ76" s="1"/>
       <c r="AK76" s="1"/>
     </row>
-    <row r="77" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="77" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
@@ -2965,7 +2964,7 @@
       <c r="AJ77" s="1"/>
       <c r="AK77" s="1"/>
     </row>
-    <row r="78" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="78" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
@@ -2992,7 +2991,7 @@
       <c r="AJ78" s="1"/>
       <c r="AK78" s="1"/>
     </row>
-    <row r="79" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="79" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
@@ -3019,7 +3018,7 @@
       <c r="AJ79" s="1"/>
       <c r="AK79" s="1"/>
     </row>
-    <row r="80" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="80" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
@@ -3046,7 +3045,7 @@
       <c r="AJ80" s="1"/>
       <c r="AK80" s="1"/>
     </row>
-    <row r="81" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="81" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
@@ -3073,7 +3072,7 @@
       <c r="AJ81" s="1"/>
       <c r="AK81" s="1"/>
     </row>
-    <row r="82" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="82" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
@@ -3100,7 +3099,7 @@
       <c r="AJ82" s="1"/>
       <c r="AK82" s="1"/>
     </row>
-    <row r="83" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="83" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
@@ -3127,7 +3126,7 @@
       <c r="AJ83" s="1"/>
       <c r="AK83" s="1"/>
     </row>
-    <row r="84" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="84" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
       <c r="O84" s="1"/>
@@ -3154,7 +3153,7 @@
       <c r="AJ84" s="1"/>
       <c r="AK84" s="1"/>
     </row>
-    <row r="85" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="85" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
       <c r="O85" s="1"/>
@@ -3181,7 +3180,7 @@
       <c r="AJ85" s="1"/>
       <c r="AK85" s="1"/>
     </row>
-    <row r="86" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="86" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
       <c r="O86" s="1"/>
@@ -3208,7 +3207,7 @@
       <c r="AJ86" s="1"/>
       <c r="AK86" s="1"/>
     </row>
-    <row r="87" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="87" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
       <c r="O87" s="1"/>
@@ -3235,7 +3234,7 @@
       <c r="AJ87" s="1"/>
       <c r="AK87" s="1"/>
     </row>
-    <row r="88" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="88" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
       <c r="O88" s="1"/>
@@ -3262,7 +3261,7 @@
       <c r="AJ88" s="1"/>
       <c r="AK88" s="1"/>
     </row>
-    <row r="89" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="89" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1"/>
@@ -3289,7 +3288,7 @@
       <c r="AJ89" s="1"/>
       <c r="AK89" s="1"/>
     </row>
-    <row r="90" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="90" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1"/>
@@ -3316,7 +3315,7 @@
       <c r="AJ90" s="1"/>
       <c r="AK90" s="1"/>
     </row>
-    <row r="91" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="91" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
       <c r="O91" s="1"/>
@@ -3343,7 +3342,7 @@
       <c r="AJ91" s="1"/>
       <c r="AK91" s="1"/>
     </row>
-    <row r="92" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="92" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
       <c r="O92" s="1"/>
@@ -3370,7 +3369,7 @@
       <c r="AJ92" s="1"/>
       <c r="AK92" s="1"/>
     </row>
-    <row r="93" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="93" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
       <c r="O93" s="1"/>
@@ -3397,7 +3396,7 @@
       <c r="AJ93" s="1"/>
       <c r="AK93" s="1"/>
     </row>
-    <row r="94" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="94" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
       <c r="O94" s="1"/>
@@ -3424,7 +3423,7 @@
       <c r="AJ94" s="1"/>
       <c r="AK94" s="1"/>
     </row>
-    <row r="95" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="95" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M95" s="1"/>
       <c r="N95" s="1"/>
       <c r="O95" s="1"/>
@@ -3451,7 +3450,7 @@
       <c r="AJ95" s="1"/>
       <c r="AK95" s="1"/>
     </row>
-    <row r="96" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="96" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
       <c r="O96" s="1"/>
@@ -3478,7 +3477,7 @@
       <c r="AJ96" s="1"/>
       <c r="AK96" s="1"/>
     </row>
-    <row r="97" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="97" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
       <c r="O97" s="1"/>
@@ -3505,7 +3504,7 @@
       <c r="AJ97" s="1"/>
       <c r="AK97" s="1"/>
     </row>
-    <row r="98" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="98" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
       <c r="O98" s="1"/>
@@ -3532,7 +3531,7 @@
       <c r="AJ98" s="1"/>
       <c r="AK98" s="1"/>
     </row>
-    <row r="99" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="99" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
       <c r="O99" s="1"/>
@@ -3559,7 +3558,7 @@
       <c r="AJ99" s="1"/>
       <c r="AK99" s="1"/>
     </row>
-    <row r="100" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="100" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
       <c r="O100" s="1"/>
@@ -3586,7 +3585,7 @@
       <c r="AJ100" s="1"/>
       <c r="AK100" s="1"/>
     </row>
-    <row r="101" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="101" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
       <c r="O101" s="1"/>
@@ -3613,7 +3612,7 @@
       <c r="AJ101" s="1"/>
       <c r="AK101" s="1"/>
     </row>
-    <row r="102" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="102" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
       <c r="O102" s="1"/>
@@ -3640,7 +3639,7 @@
       <c r="AJ102" s="1"/>
       <c r="AK102" s="1"/>
     </row>
-    <row r="103" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="103" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
       <c r="O103" s="1"/>
@@ -3667,7 +3666,7 @@
       <c r="AJ103" s="1"/>
       <c r="AK103" s="1"/>
     </row>
-    <row r="104" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="104" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
       <c r="O104" s="1"/>
@@ -3694,7 +3693,7 @@
       <c r="AJ104" s="1"/>
       <c r="AK104" s="1"/>
     </row>
-    <row r="105" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="105" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M105" s="1"/>
       <c r="N105" s="1"/>
       <c r="O105" s="1"/>
@@ -3721,7 +3720,7 @@
       <c r="AJ105" s="1"/>
       <c r="AK105" s="1"/>
     </row>
-    <row r="106" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="106" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
       <c r="O106" s="1"/>
@@ -3748,7 +3747,7 @@
       <c r="AJ106" s="1"/>
       <c r="AK106" s="1"/>
     </row>
-    <row r="107" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="107" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M107" s="1"/>
       <c r="N107" s="1"/>
       <c r="O107" s="1"/>
@@ -3775,7 +3774,7 @@
       <c r="AJ107" s="1"/>
       <c r="AK107" s="1"/>
     </row>
-    <row r="108" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="108" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M108" s="1"/>
       <c r="N108" s="1"/>
       <c r="O108" s="1"/>
@@ -3802,7 +3801,7 @@
       <c r="AJ108" s="1"/>
       <c r="AK108" s="1"/>
     </row>
-    <row r="109" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="109" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M109" s="1"/>
       <c r="N109" s="1"/>
       <c r="O109" s="1"/>
@@ -3829,7 +3828,7 @@
       <c r="AJ109" s="1"/>
       <c r="AK109" s="1"/>
     </row>
-    <row r="110" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="110" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M110" s="1"/>
       <c r="N110" s="1"/>
       <c r="O110" s="1"/>
@@ -3856,7 +3855,7 @@
       <c r="AJ110" s="1"/>
       <c r="AK110" s="1"/>
     </row>
-    <row r="111" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="111" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M111" s="1"/>
       <c r="N111" s="1"/>
       <c r="O111" s="1"/>
@@ -3883,7 +3882,7 @@
       <c r="AJ111" s="1"/>
       <c r="AK111" s="1"/>
     </row>
-    <row r="112" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="112" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M112" s="1"/>
       <c r="N112" s="1"/>
       <c r="O112" s="1"/>
@@ -3910,7 +3909,7 @@
       <c r="AJ112" s="1"/>
       <c r="AK112" s="1"/>
     </row>
-    <row r="113" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="113" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M113" s="1"/>
       <c r="N113" s="1"/>
       <c r="O113" s="1"/>
@@ -3937,7 +3936,7 @@
       <c r="AJ113" s="1"/>
       <c r="AK113" s="1"/>
     </row>
-    <row r="114" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="114" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M114" s="1"/>
       <c r="N114" s="1"/>
       <c r="O114" s="1"/>
@@ -3964,7 +3963,7 @@
       <c r="AJ114" s="1"/>
       <c r="AK114" s="1"/>
     </row>
-    <row r="115" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="115" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M115" s="1"/>
       <c r="N115" s="1"/>
       <c r="O115" s="1"/>
@@ -3991,7 +3990,7 @@
       <c r="AJ115" s="1"/>
       <c r="AK115" s="1"/>
     </row>
-    <row r="116" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="116" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M116" s="1"/>
       <c r="N116" s="1"/>
       <c r="O116" s="1"/>
@@ -4018,7 +4017,7 @@
       <c r="AJ116" s="1"/>
       <c r="AK116" s="1"/>
     </row>
-    <row r="117" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="117" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M117" s="1"/>
       <c r="N117" s="1"/>
       <c r="O117" s="1"/>
@@ -4045,7 +4044,7 @@
       <c r="AJ117" s="1"/>
       <c r="AK117" s="1"/>
     </row>
-    <row r="118" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="118" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M118" s="1"/>
       <c r="N118" s="1"/>
       <c r="O118" s="1"/>
@@ -4072,7 +4071,7 @@
       <c r="AJ118" s="1"/>
       <c r="AK118" s="1"/>
     </row>
-    <row r="119" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="119" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M119" s="1"/>
       <c r="N119" s="1"/>
       <c r="O119" s="1"/>
@@ -4099,7 +4098,7 @@
       <c r="AJ119" s="1"/>
       <c r="AK119" s="1"/>
     </row>
-    <row r="120" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="120" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M120" s="1"/>
       <c r="N120" s="1"/>
       <c r="O120" s="1"/>
@@ -4126,7 +4125,7 @@
       <c r="AJ120" s="1"/>
       <c r="AK120" s="1"/>
     </row>
-    <row r="121" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="121" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M121" s="1"/>
       <c r="N121" s="1"/>
       <c r="O121" s="1"/>
@@ -4153,7 +4152,7 @@
       <c r="AJ121" s="1"/>
       <c r="AK121" s="1"/>
     </row>
-    <row r="122" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="122" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M122" s="1"/>
       <c r="N122" s="1"/>
       <c r="O122" s="1"/>
@@ -4180,7 +4179,7 @@
       <c r="AJ122" s="1"/>
       <c r="AK122" s="1"/>
     </row>
-    <row r="123" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="123" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M123" s="1"/>
       <c r="N123" s="1"/>
       <c r="O123" s="1"/>
@@ -4207,7 +4206,7 @@
       <c r="AJ123" s="1"/>
       <c r="AK123" s="1"/>
     </row>
-    <row r="124" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="124" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M124" s="1"/>
       <c r="N124" s="1"/>
       <c r="O124" s="1"/>
@@ -4234,7 +4233,7 @@
       <c r="AJ124" s="1"/>
       <c r="AK124" s="1"/>
     </row>
-    <row r="125" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="125" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M125" s="1"/>
       <c r="N125" s="1"/>
       <c r="O125" s="1"/>
@@ -4261,7 +4260,7 @@
       <c r="AJ125" s="1"/>
       <c r="AK125" s="1"/>
     </row>
-    <row r="126" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="126" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M126" s="1"/>
       <c r="N126" s="1"/>
       <c r="O126" s="1"/>
@@ -4288,7 +4287,7 @@
       <c r="AJ126" s="1"/>
       <c r="AK126" s="1"/>
     </row>
-    <row r="127" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="127" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
       <c r="O127" s="1"/>
@@ -4315,7 +4314,7 @@
       <c r="AJ127" s="1"/>
       <c r="AK127" s="1"/>
     </row>
-    <row r="128" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="128" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M128" s="1"/>
       <c r="N128" s="1"/>
       <c r="O128" s="1"/>
@@ -4342,7 +4341,7 @@
       <c r="AJ128" s="1"/>
       <c r="AK128" s="1"/>
     </row>
-    <row r="129" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="129" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M129" s="1"/>
       <c r="N129" s="1"/>
       <c r="O129" s="1"/>
@@ -4369,7 +4368,7 @@
       <c r="AJ129" s="1"/>
       <c r="AK129" s="1"/>
     </row>
-    <row r="130" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="130" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M130" s="1"/>
       <c r="N130" s="1"/>
       <c r="O130" s="1"/>
@@ -4396,7 +4395,7 @@
       <c r="AJ130" s="1"/>
       <c r="AK130" s="1"/>
     </row>
-    <row r="131" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="131" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M131" s="1"/>
       <c r="N131" s="1"/>
       <c r="O131" s="1"/>
@@ -4423,7 +4422,7 @@
       <c r="AJ131" s="1"/>
       <c r="AK131" s="1"/>
     </row>
-    <row r="132" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="132" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M132" s="1"/>
       <c r="N132" s="1"/>
       <c r="O132" s="1"/>
@@ -4450,7 +4449,7 @@
       <c r="AJ132" s="1"/>
       <c r="AK132" s="1"/>
     </row>
-    <row r="133" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="133" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M133" s="1"/>
       <c r="N133" s="1"/>
       <c r="O133" s="1"/>
@@ -4477,7 +4476,7 @@
       <c r="AJ133" s="1"/>
       <c r="AK133" s="1"/>
     </row>
-    <row r="134" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="134" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M134" s="1"/>
       <c r="N134" s="1"/>
       <c r="O134" s="1"/>
@@ -4504,7 +4503,7 @@
       <c r="AJ134" s="1"/>
       <c r="AK134" s="1"/>
     </row>
-    <row r="135" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="135" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M135" s="1"/>
       <c r="N135" s="1"/>
       <c r="O135" s="1"/>
@@ -4531,7 +4530,7 @@
       <c r="AJ135" s="1"/>
       <c r="AK135" s="1"/>
     </row>
-    <row r="136" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="136" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M136" s="1"/>
       <c r="N136" s="1"/>
       <c r="O136" s="1"/>
@@ -4558,7 +4557,7 @@
       <c r="AJ136" s="1"/>
       <c r="AK136" s="1"/>
     </row>
-    <row r="137" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="137" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M137" s="1"/>
       <c r="N137" s="1"/>
       <c r="O137" s="1"/>
@@ -4585,7 +4584,7 @@
       <c r="AJ137" s="1"/>
       <c r="AK137" s="1"/>
     </row>
-    <row r="138" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="138" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M138" s="1"/>
       <c r="N138" s="1"/>
       <c r="O138" s="1"/>
@@ -4612,7 +4611,7 @@
       <c r="AJ138" s="1"/>
       <c r="AK138" s="1"/>
     </row>
-    <row r="139" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="139" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M139" s="1"/>
       <c r="N139" s="1"/>
       <c r="O139" s="1"/>
@@ -4639,7 +4638,7 @@
       <c r="AJ139" s="1"/>
       <c r="AK139" s="1"/>
     </row>
-    <row r="140" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="140" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M140" s="1"/>
       <c r="N140" s="1"/>
       <c r="O140" s="1"/>
@@ -4666,7 +4665,7 @@
       <c r="AJ140" s="1"/>
       <c r="AK140" s="1"/>
     </row>
-    <row r="141" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="141" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M141" s="1"/>
       <c r="N141" s="1"/>
       <c r="O141" s="1"/>
@@ -4693,7 +4692,7 @@
       <c r="AJ141" s="1"/>
       <c r="AK141" s="1"/>
     </row>
-    <row r="142" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="142" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M142" s="1"/>
       <c r="N142" s="1"/>
       <c r="O142" s="1"/>
@@ -4720,7 +4719,7 @@
       <c r="AJ142" s="1"/>
       <c r="AK142" s="1"/>
     </row>
-    <row r="143" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="143" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M143" s="1"/>
       <c r="N143" s="1"/>
       <c r="O143" s="1"/>
@@ -4747,7 +4746,7 @@
       <c r="AJ143" s="1"/>
       <c r="AK143" s="1"/>
     </row>
-    <row r="144" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="144" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M144" s="1"/>
       <c r="N144" s="1"/>
       <c r="O144" s="1"/>
@@ -4774,7 +4773,7 @@
       <c r="AJ144" s="1"/>
       <c r="AK144" s="1"/>
     </row>
-    <row r="145" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="145" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M145" s="1"/>
       <c r="N145" s="1"/>
       <c r="O145" s="1"/>
@@ -4801,7 +4800,7 @@
       <c r="AJ145" s="1"/>
       <c r="AK145" s="1"/>
     </row>
-    <row r="146" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="146" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M146" s="1"/>
       <c r="N146" s="1"/>
       <c r="O146" s="1"/>
@@ -4828,7 +4827,7 @@
       <c r="AJ146" s="1"/>
       <c r="AK146" s="1"/>
     </row>
-    <row r="147" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="147" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M147" s="1"/>
       <c r="N147" s="1"/>
       <c r="O147" s="1"/>
@@ -4855,7 +4854,7 @@
       <c r="AJ147" s="1"/>
       <c r="AK147" s="1"/>
     </row>
-    <row r="148" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="148" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M148" s="1"/>
       <c r="N148" s="1"/>
       <c r="O148" s="1"/>
@@ -4882,7 +4881,7 @@
       <c r="AJ148" s="1"/>
       <c r="AK148" s="1"/>
     </row>
-    <row r="149" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="149" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M149" s="1"/>
       <c r="N149" s="1"/>
       <c r="O149" s="1"/>
@@ -4909,7 +4908,7 @@
       <c r="AJ149" s="1"/>
       <c r="AK149" s="1"/>
     </row>
-    <row r="150" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="150" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M150" s="1"/>
       <c r="N150" s="1"/>
       <c r="O150" s="1"/>
@@ -4936,7 +4935,7 @@
       <c r="AJ150" s="1"/>
       <c r="AK150" s="1"/>
     </row>
-    <row r="151" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="151" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M151" s="1"/>
       <c r="N151" s="1"/>
       <c r="O151" s="1"/>
@@ -4963,7 +4962,7 @@
       <c r="AJ151" s="1"/>
       <c r="AK151" s="1"/>
     </row>
-    <row r="152" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="152" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M152" s="1"/>
       <c r="N152" s="1"/>
       <c r="O152" s="1"/>
@@ -4990,7 +4989,7 @@
       <c r="AJ152" s="1"/>
       <c r="AK152" s="1"/>
     </row>
-    <row r="153" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="153" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M153" s="1"/>
       <c r="N153" s="1"/>
       <c r="O153" s="1"/>
@@ -5017,7 +5016,7 @@
       <c r="AJ153" s="1"/>
       <c r="AK153" s="1"/>
     </row>
-    <row r="154" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="154" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M154" s="1"/>
       <c r="N154" s="1"/>
       <c r="O154" s="1"/>
@@ -5044,7 +5043,7 @@
       <c r="AJ154" s="1"/>
       <c r="AK154" s="1"/>
     </row>
-    <row r="155" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="155" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M155" s="1"/>
       <c r="N155" s="1"/>
       <c r="O155" s="1"/>
@@ -5071,7 +5070,7 @@
       <c r="AJ155" s="1"/>
       <c r="AK155" s="1"/>
     </row>
-    <row r="156" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="156" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M156" s="1"/>
       <c r="N156" s="1"/>
       <c r="O156" s="1"/>
@@ -5098,7 +5097,7 @@
       <c r="AJ156" s="1"/>
       <c r="AK156" s="1"/>
     </row>
-    <row r="157" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="157" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M157" s="1"/>
       <c r="N157" s="1"/>
       <c r="O157" s="1"/>
@@ -5125,7 +5124,7 @@
       <c r="AJ157" s="1"/>
       <c r="AK157" s="1"/>
     </row>
-    <row r="158" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="158" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M158" s="1"/>
       <c r="N158" s="1"/>
       <c r="O158" s="1"/>
@@ -5152,7 +5151,7 @@
       <c r="AJ158" s="1"/>
       <c r="AK158" s="1"/>
     </row>
-    <row r="159" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="159" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M159" s="1"/>
       <c r="N159" s="1"/>
       <c r="O159" s="1"/>
@@ -5179,7 +5178,7 @@
       <c r="AJ159" s="1"/>
       <c r="AK159" s="1"/>
     </row>
-    <row r="160" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="160" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M160" s="1"/>
       <c r="N160" s="1"/>
       <c r="O160" s="1"/>
@@ -5206,7 +5205,7 @@
       <c r="AJ160" s="1"/>
       <c r="AK160" s="1"/>
     </row>
-    <row r="161" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="161" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M161" s="1"/>
       <c r="N161" s="1"/>
       <c r="O161" s="1"/>
@@ -5235,16 +5234,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D11:F14"/>
-    <mergeCell ref="G11:I14"/>
-    <mergeCell ref="J11:L14"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="A3:C6"/>
-    <mergeCell ref="D3:F6"/>
-    <mergeCell ref="G3:I6"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="M3:O6"/>
     <mergeCell ref="M7:O10"/>
@@ -5261,6 +5250,16 @@
     <mergeCell ref="G7:I10"/>
     <mergeCell ref="J7:L10"/>
     <mergeCell ref="A11:C14"/>
+    <mergeCell ref="D11:F14"/>
+    <mergeCell ref="G11:I14"/>
+    <mergeCell ref="J11:L14"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="A3:C6"/>
+    <mergeCell ref="D3:F6"/>
+    <mergeCell ref="G3:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5268,18 +5267,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5429,6 +5428,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A7B2E4-0806-468A-9362-8AC839DA2BE7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -5440,14 +5447,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
member 1:use case diagram feito e atualizei o backlog
</commit_message>
<xml_diff>
--- a/scrum/Phase1/Sprint1/Sprint_backlog.xlsx
+++ b/scrum/Phase1/Sprint1/Sprint_backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\SE2122_57464_58763_57677_58125_63764\scrum\Phase1\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nova pasta\SE2122_57464_58763_57677_58125_63764\scrum\Phase1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A872BD-59A9-48E9-9DA7-D284A7E83815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A2FEFB-194E-47F9-BEE5-A22C9A66720A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
+    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -91,10 +91,6 @@
 Member 1: finished pattern detection Member 4: finished pattern detection</t>
   </si>
   <si>
-    <t>Member 5: finished Reviews.
-Member 2: finished Reviews. Member 4: finished Reviews.</t>
-  </si>
-  <si>
     <t>Member 3: model package
 Member 4: do the MOOD metrics set, analyse the result and make a report.</t>
   </si>
@@ -105,9 +101,6 @@
 </t>
   </si>
   <si>
-    <t>Member 3:  reviewing the design patterns</t>
-  </si>
-  <si>
     <t xml:space="preserve">Member 5: finished doing the metrics
 Member 1: finished doing the metrics
 Member 2: finished doing the metrics Member 4: finished doing the metrics
@@ -115,21 +108,26 @@
 </t>
   </si>
   <si>
-    <t>Member 3:  reviewing the metrics</t>
+    <t>Member 1: gui package
+Member 3: model package
+Member 4: preferences package</t>
+  </si>
+  <si>
+    <t>Member 5: finished Reviews.
+Member 2: finished Reviews. Member 4: finished Reviews.
+Member 1: finished Reviews.</t>
+  </si>
+  <si>
+    <t>Member 4: making diagrams</t>
   </si>
   <si>
     <t>Member 5: finished Use case diagrams
-Member 2: finished Use case diagrams</t>
+Member 2: finished Use case diagrams
+Member 1: finished Use case diagrams
+Member 3: making diagrams</t>
   </si>
   <si>
-    <t>Member 3: making diagrams
-Member 1: making diagram
-Member 4: making diagrams</t>
-  </si>
-  <si>
-    <t>Member 1: gui package
-Member 3: model package
-Member 4: preferences package</t>
+    <t>Member 3: Reviewing.</t>
   </si>
 </sst>
 </file>
@@ -252,14 +250,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -267,11 +268,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -280,12 +284,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -607,34 +605,34 @@
   <dimension ref="A1:AL161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:F10"/>
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="46.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:38" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -659,32 +657,32 @@
       <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
     </row>
-    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="6" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="6" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="6" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="6" t="s">
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -708,26 +706,26 @@
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="4" t="s">
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N3" s="5"/>
@@ -755,19 +753,19 @@
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -794,19 +792,19 @@
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
@@ -833,19 +831,19 @@
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
     </row>
-    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
+    <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
@@ -872,23 +870,23 @@
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
     </row>
-    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="8" t="s">
-        <v>23</v>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="3" t="s">
+        <v>18</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="4" t="s">
-        <v>22</v>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="6" t="s">
         <v>21</v>
       </c>
       <c r="K7" s="5"/>
@@ -919,10 +917,10 @@
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -958,10 +956,10 @@
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -997,10 +995,10 @@
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
     </row>
-    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+    <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -1014,7 +1012,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
+      <c r="Q10" s="2"/>
       <c r="R10" s="1"/>
       <c r="S10" s="2"/>
       <c r="T10" s="1"/>
@@ -1036,29 +1034,27 @@
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="4" t="s">
-        <v>17</v>
+      <c r="M11" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -1069,7 +1065,7 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
+      <c r="W11" s="2"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
@@ -1085,7 +1081,7 @@
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1124,7 +1120,7 @@
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1163,7 +1159,7 @@
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
     </row>
-    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1202,29 +1198,29 @@
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="8" t="s">
-        <v>16</v>
+      <c r="D15" s="3" t="s">
+        <v>15</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="4" t="s">
-        <v>20</v>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="4" t="s">
-        <v>19</v>
+      <c r="J15" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
-      <c r="M15" s="4" t="s">
-        <v>15</v>
+      <c r="M15" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
@@ -1251,7 +1247,7 @@
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1290,7 +1286,7 @@
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1329,7 +1325,7 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
     </row>
-    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1368,7 +1364,7 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1395,7 +1391,7 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1422,7 +1418,7 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -1449,7 +1445,7 @@
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -1476,7 +1472,7 @@
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -1503,7 +1499,7 @@
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -1530,7 +1526,7 @@
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -1557,7 +1553,7 @@
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -1584,7 +1580,7 @@
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -1611,7 +1607,7 @@
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -1638,7 +1634,7 @@
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
@@ -1665,7 +1661,7 @@
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -1692,7 +1688,7 @@
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -1719,7 +1715,7 @@
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -1746,7 +1742,7 @@
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
     </row>
-    <row r="33" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -1773,7 +1769,7 @@
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
     </row>
-    <row r="34" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -1800,7 +1796,7 @@
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
     </row>
-    <row r="35" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -1827,7 +1823,7 @@
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
     </row>
-    <row r="36" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
@@ -1854,7 +1850,7 @@
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
     </row>
-    <row r="37" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="37" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
@@ -1881,7 +1877,7 @@
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
     </row>
-    <row r="38" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
@@ -1908,7 +1904,7 @@
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
     </row>
-    <row r="39" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
@@ -1935,7 +1931,7 @@
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
     </row>
-    <row r="40" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="40" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
@@ -1962,7 +1958,7 @@
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
     </row>
-    <row r="41" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="41" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
@@ -1989,7 +1985,7 @@
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
     </row>
-    <row r="42" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="42" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
@@ -2016,7 +2012,7 @@
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
     </row>
-    <row r="43" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="43" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
@@ -2043,7 +2039,7 @@
       <c r="AJ43" s="1"/>
       <c r="AK43" s="1"/>
     </row>
-    <row r="44" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="44" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
@@ -2070,7 +2066,7 @@
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
     </row>
-    <row r="45" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="45" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
@@ -2097,7 +2093,7 @@
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
     </row>
-    <row r="46" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="46" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
@@ -2124,7 +2120,7 @@
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
     </row>
-    <row r="47" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="47" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
@@ -2151,7 +2147,7 @@
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
     </row>
-    <row r="48" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="48" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
@@ -2178,7 +2174,7 @@
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
     </row>
-    <row r="49" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="49" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
@@ -2205,7 +2201,7 @@
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
     </row>
-    <row r="50" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="50" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
@@ -2232,7 +2228,7 @@
       <c r="AJ50" s="1"/>
       <c r="AK50" s="1"/>
     </row>
-    <row r="51" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="51" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
@@ -2259,7 +2255,7 @@
       <c r="AJ51" s="1"/>
       <c r="AK51" s="1"/>
     </row>
-    <row r="52" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="52" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
@@ -2286,7 +2282,7 @@
       <c r="AJ52" s="1"/>
       <c r="AK52" s="1"/>
     </row>
-    <row r="53" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="53" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
@@ -2313,7 +2309,7 @@
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
     </row>
-    <row r="54" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="54" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
@@ -2340,7 +2336,7 @@
       <c r="AJ54" s="1"/>
       <c r="AK54" s="1"/>
     </row>
-    <row r="55" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="55" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
@@ -2367,7 +2363,7 @@
       <c r="AJ55" s="1"/>
       <c r="AK55" s="1"/>
     </row>
-    <row r="56" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="56" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
@@ -2394,7 +2390,7 @@
       <c r="AJ56" s="1"/>
       <c r="AK56" s="1"/>
     </row>
-    <row r="57" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="57" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
@@ -2421,7 +2417,7 @@
       <c r="AJ57" s="1"/>
       <c r="AK57" s="1"/>
     </row>
-    <row r="58" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="58" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
@@ -2448,7 +2444,7 @@
       <c r="AJ58" s="1"/>
       <c r="AK58" s="1"/>
     </row>
-    <row r="59" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="59" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
@@ -2475,7 +2471,7 @@
       <c r="AJ59" s="1"/>
       <c r="AK59" s="1"/>
     </row>
-    <row r="60" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="60" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
@@ -2502,7 +2498,7 @@
       <c r="AJ60" s="1"/>
       <c r="AK60" s="1"/>
     </row>
-    <row r="61" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="61" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
@@ -2529,7 +2525,7 @@
       <c r="AJ61" s="1"/>
       <c r="AK61" s="1"/>
     </row>
-    <row r="62" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="62" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
@@ -2556,7 +2552,7 @@
       <c r="AJ62" s="1"/>
       <c r="AK62" s="1"/>
     </row>
-    <row r="63" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="63" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
@@ -2583,7 +2579,7 @@
       <c r="AJ63" s="1"/>
       <c r="AK63" s="1"/>
     </row>
-    <row r="64" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="64" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
@@ -2610,7 +2606,7 @@
       <c r="AJ64" s="1"/>
       <c r="AK64" s="1"/>
     </row>
-    <row r="65" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="65" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
@@ -2637,7 +2633,7 @@
       <c r="AJ65" s="1"/>
       <c r="AK65" s="1"/>
     </row>
-    <row r="66" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="66" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
       <c r="O66" s="1"/>
@@ -2664,7 +2660,7 @@
       <c r="AJ66" s="1"/>
       <c r="AK66" s="1"/>
     </row>
-    <row r="67" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="67" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
@@ -2691,7 +2687,7 @@
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
     </row>
-    <row r="68" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="68" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
@@ -2718,7 +2714,7 @@
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
     </row>
-    <row r="69" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="69" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
@@ -2745,7 +2741,7 @@
       <c r="AJ69" s="1"/>
       <c r="AK69" s="1"/>
     </row>
-    <row r="70" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="70" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
@@ -2772,7 +2768,7 @@
       <c r="AJ70" s="1"/>
       <c r="AK70" s="1"/>
     </row>
-    <row r="71" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="71" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
@@ -2799,7 +2795,7 @@
       <c r="AJ71" s="1"/>
       <c r="AK71" s="1"/>
     </row>
-    <row r="72" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="72" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
@@ -2826,7 +2822,7 @@
       <c r="AJ72" s="1"/>
       <c r="AK72" s="1"/>
     </row>
-    <row r="73" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="73" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
@@ -2853,7 +2849,7 @@
       <c r="AJ73" s="1"/>
       <c r="AK73" s="1"/>
     </row>
-    <row r="74" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="74" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
@@ -2880,7 +2876,7 @@
       <c r="AJ74" s="1"/>
       <c r="AK74" s="1"/>
     </row>
-    <row r="75" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="75" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
@@ -2907,7 +2903,7 @@
       <c r="AJ75" s="1"/>
       <c r="AK75" s="1"/>
     </row>
-    <row r="76" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="76" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
@@ -2934,7 +2930,7 @@
       <c r="AJ76" s="1"/>
       <c r="AK76" s="1"/>
     </row>
-    <row r="77" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="77" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
@@ -2961,7 +2957,7 @@
       <c r="AJ77" s="1"/>
       <c r="AK77" s="1"/>
     </row>
-    <row r="78" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="78" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
@@ -2988,7 +2984,7 @@
       <c r="AJ78" s="1"/>
       <c r="AK78" s="1"/>
     </row>
-    <row r="79" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="79" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
@@ -3015,7 +3011,7 @@
       <c r="AJ79" s="1"/>
       <c r="AK79" s="1"/>
     </row>
-    <row r="80" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="80" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
@@ -3042,7 +3038,7 @@
       <c r="AJ80" s="1"/>
       <c r="AK80" s="1"/>
     </row>
-    <row r="81" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="81" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
@@ -3069,7 +3065,7 @@
       <c r="AJ81" s="1"/>
       <c r="AK81" s="1"/>
     </row>
-    <row r="82" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="82" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
@@ -3096,7 +3092,7 @@
       <c r="AJ82" s="1"/>
       <c r="AK82" s="1"/>
     </row>
-    <row r="83" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="83" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
@@ -3123,7 +3119,7 @@
       <c r="AJ83" s="1"/>
       <c r="AK83" s="1"/>
     </row>
-    <row r="84" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="84" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
       <c r="O84" s="1"/>
@@ -3150,7 +3146,7 @@
       <c r="AJ84" s="1"/>
       <c r="AK84" s="1"/>
     </row>
-    <row r="85" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="85" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
       <c r="O85" s="1"/>
@@ -3177,7 +3173,7 @@
       <c r="AJ85" s="1"/>
       <c r="AK85" s="1"/>
     </row>
-    <row r="86" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="86" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
       <c r="O86" s="1"/>
@@ -3204,7 +3200,7 @@
       <c r="AJ86" s="1"/>
       <c r="AK86" s="1"/>
     </row>
-    <row r="87" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="87" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
       <c r="O87" s="1"/>
@@ -3231,7 +3227,7 @@
       <c r="AJ87" s="1"/>
       <c r="AK87" s="1"/>
     </row>
-    <row r="88" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="88" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
       <c r="O88" s="1"/>
@@ -3258,7 +3254,7 @@
       <c r="AJ88" s="1"/>
       <c r="AK88" s="1"/>
     </row>
-    <row r="89" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="89" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1"/>
@@ -3285,7 +3281,7 @@
       <c r="AJ89" s="1"/>
       <c r="AK89" s="1"/>
     </row>
-    <row r="90" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="90" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1"/>
@@ -3312,7 +3308,7 @@
       <c r="AJ90" s="1"/>
       <c r="AK90" s="1"/>
     </row>
-    <row r="91" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="91" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
       <c r="O91" s="1"/>
@@ -3339,7 +3335,7 @@
       <c r="AJ91" s="1"/>
       <c r="AK91" s="1"/>
     </row>
-    <row r="92" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="92" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
       <c r="O92" s="1"/>
@@ -3366,7 +3362,7 @@
       <c r="AJ92" s="1"/>
       <c r="AK92" s="1"/>
     </row>
-    <row r="93" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="93" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
       <c r="O93" s="1"/>
@@ -3393,7 +3389,7 @@
       <c r="AJ93" s="1"/>
       <c r="AK93" s="1"/>
     </row>
-    <row r="94" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="94" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
       <c r="O94" s="1"/>
@@ -3420,7 +3416,7 @@
       <c r="AJ94" s="1"/>
       <c r="AK94" s="1"/>
     </row>
-    <row r="95" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="95" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M95" s="1"/>
       <c r="N95" s="1"/>
       <c r="O95" s="1"/>
@@ -3447,7 +3443,7 @@
       <c r="AJ95" s="1"/>
       <c r="AK95" s="1"/>
     </row>
-    <row r="96" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="96" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
       <c r="O96" s="1"/>
@@ -3474,7 +3470,7 @@
       <c r="AJ96" s="1"/>
       <c r="AK96" s="1"/>
     </row>
-    <row r="97" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="97" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
       <c r="O97" s="1"/>
@@ -3501,7 +3497,7 @@
       <c r="AJ97" s="1"/>
       <c r="AK97" s="1"/>
     </row>
-    <row r="98" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="98" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
       <c r="O98" s="1"/>
@@ -3528,7 +3524,7 @@
       <c r="AJ98" s="1"/>
       <c r="AK98" s="1"/>
     </row>
-    <row r="99" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="99" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
       <c r="O99" s="1"/>
@@ -3555,7 +3551,7 @@
       <c r="AJ99" s="1"/>
       <c r="AK99" s="1"/>
     </row>
-    <row r="100" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="100" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
       <c r="O100" s="1"/>
@@ -3582,7 +3578,7 @@
       <c r="AJ100" s="1"/>
       <c r="AK100" s="1"/>
     </row>
-    <row r="101" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="101" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
       <c r="O101" s="1"/>
@@ -3609,7 +3605,7 @@
       <c r="AJ101" s="1"/>
       <c r="AK101" s="1"/>
     </row>
-    <row r="102" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="102" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
       <c r="O102" s="1"/>
@@ -3636,7 +3632,7 @@
       <c r="AJ102" s="1"/>
       <c r="AK102" s="1"/>
     </row>
-    <row r="103" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="103" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
       <c r="O103" s="1"/>
@@ -3663,7 +3659,7 @@
       <c r="AJ103" s="1"/>
       <c r="AK103" s="1"/>
     </row>
-    <row r="104" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="104" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
       <c r="O104" s="1"/>
@@ -3690,7 +3686,7 @@
       <c r="AJ104" s="1"/>
       <c r="AK104" s="1"/>
     </row>
-    <row r="105" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="105" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M105" s="1"/>
       <c r="N105" s="1"/>
       <c r="O105" s="1"/>
@@ -3717,7 +3713,7 @@
       <c r="AJ105" s="1"/>
       <c r="AK105" s="1"/>
     </row>
-    <row r="106" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="106" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
       <c r="O106" s="1"/>
@@ -3744,7 +3740,7 @@
       <c r="AJ106" s="1"/>
       <c r="AK106" s="1"/>
     </row>
-    <row r="107" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="107" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M107" s="1"/>
       <c r="N107" s="1"/>
       <c r="O107" s="1"/>
@@ -3771,7 +3767,7 @@
       <c r="AJ107" s="1"/>
       <c r="AK107" s="1"/>
     </row>
-    <row r="108" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="108" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M108" s="1"/>
       <c r="N108" s="1"/>
       <c r="O108" s="1"/>
@@ -3798,7 +3794,7 @@
       <c r="AJ108" s="1"/>
       <c r="AK108" s="1"/>
     </row>
-    <row r="109" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="109" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M109" s="1"/>
       <c r="N109" s="1"/>
       <c r="O109" s="1"/>
@@ -3825,7 +3821,7 @@
       <c r="AJ109" s="1"/>
       <c r="AK109" s="1"/>
     </row>
-    <row r="110" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="110" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M110" s="1"/>
       <c r="N110" s="1"/>
       <c r="O110" s="1"/>
@@ -3852,7 +3848,7 @@
       <c r="AJ110" s="1"/>
       <c r="AK110" s="1"/>
     </row>
-    <row r="111" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="111" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M111" s="1"/>
       <c r="N111" s="1"/>
       <c r="O111" s="1"/>
@@ -3879,7 +3875,7 @@
       <c r="AJ111" s="1"/>
       <c r="AK111" s="1"/>
     </row>
-    <row r="112" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="112" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M112" s="1"/>
       <c r="N112" s="1"/>
       <c r="O112" s="1"/>
@@ -3906,7 +3902,7 @@
       <c r="AJ112" s="1"/>
       <c r="AK112" s="1"/>
     </row>
-    <row r="113" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="113" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M113" s="1"/>
       <c r="N113" s="1"/>
       <c r="O113" s="1"/>
@@ -3933,7 +3929,7 @@
       <c r="AJ113" s="1"/>
       <c r="AK113" s="1"/>
     </row>
-    <row r="114" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="114" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M114" s="1"/>
       <c r="N114" s="1"/>
       <c r="O114" s="1"/>
@@ -3960,7 +3956,7 @@
       <c r="AJ114" s="1"/>
       <c r="AK114" s="1"/>
     </row>
-    <row r="115" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="115" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M115" s="1"/>
       <c r="N115" s="1"/>
       <c r="O115" s="1"/>
@@ -3987,7 +3983,7 @@
       <c r="AJ115" s="1"/>
       <c r="AK115" s="1"/>
     </row>
-    <row r="116" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="116" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M116" s="1"/>
       <c r="N116" s="1"/>
       <c r="O116" s="1"/>
@@ -4014,7 +4010,7 @@
       <c r="AJ116" s="1"/>
       <c r="AK116" s="1"/>
     </row>
-    <row r="117" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="117" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M117" s="1"/>
       <c r="N117" s="1"/>
       <c r="O117" s="1"/>
@@ -4041,7 +4037,7 @@
       <c r="AJ117" s="1"/>
       <c r="AK117" s="1"/>
     </row>
-    <row r="118" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="118" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M118" s="1"/>
       <c r="N118" s="1"/>
       <c r="O118" s="1"/>
@@ -4068,7 +4064,7 @@
       <c r="AJ118" s="1"/>
       <c r="AK118" s="1"/>
     </row>
-    <row r="119" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="119" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M119" s="1"/>
       <c r="N119" s="1"/>
       <c r="O119" s="1"/>
@@ -4095,7 +4091,7 @@
       <c r="AJ119" s="1"/>
       <c r="AK119" s="1"/>
     </row>
-    <row r="120" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="120" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M120" s="1"/>
       <c r="N120" s="1"/>
       <c r="O120" s="1"/>
@@ -4122,7 +4118,7 @@
       <c r="AJ120" s="1"/>
       <c r="AK120" s="1"/>
     </row>
-    <row r="121" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="121" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M121" s="1"/>
       <c r="N121" s="1"/>
       <c r="O121" s="1"/>
@@ -4149,7 +4145,7 @@
       <c r="AJ121" s="1"/>
       <c r="AK121" s="1"/>
     </row>
-    <row r="122" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="122" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M122" s="1"/>
       <c r="N122" s="1"/>
       <c r="O122" s="1"/>
@@ -4176,7 +4172,7 @@
       <c r="AJ122" s="1"/>
       <c r="AK122" s="1"/>
     </row>
-    <row r="123" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="123" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M123" s="1"/>
       <c r="N123" s="1"/>
       <c r="O123" s="1"/>
@@ -4203,7 +4199,7 @@
       <c r="AJ123" s="1"/>
       <c r="AK123" s="1"/>
     </row>
-    <row r="124" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="124" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M124" s="1"/>
       <c r="N124" s="1"/>
       <c r="O124" s="1"/>
@@ -4230,7 +4226,7 @@
       <c r="AJ124" s="1"/>
       <c r="AK124" s="1"/>
     </row>
-    <row r="125" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="125" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M125" s="1"/>
       <c r="N125" s="1"/>
       <c r="O125" s="1"/>
@@ -4257,7 +4253,7 @@
       <c r="AJ125" s="1"/>
       <c r="AK125" s="1"/>
     </row>
-    <row r="126" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="126" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M126" s="1"/>
       <c r="N126" s="1"/>
       <c r="O126" s="1"/>
@@ -4284,7 +4280,7 @@
       <c r="AJ126" s="1"/>
       <c r="AK126" s="1"/>
     </row>
-    <row r="127" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="127" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
       <c r="O127" s="1"/>
@@ -4311,7 +4307,7 @@
       <c r="AJ127" s="1"/>
       <c r="AK127" s="1"/>
     </row>
-    <row r="128" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="128" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M128" s="1"/>
       <c r="N128" s="1"/>
       <c r="O128" s="1"/>
@@ -4338,7 +4334,7 @@
       <c r="AJ128" s="1"/>
       <c r="AK128" s="1"/>
     </row>
-    <row r="129" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="129" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M129" s="1"/>
       <c r="N129" s="1"/>
       <c r="O129" s="1"/>
@@ -4365,7 +4361,7 @@
       <c r="AJ129" s="1"/>
       <c r="AK129" s="1"/>
     </row>
-    <row r="130" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="130" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M130" s="1"/>
       <c r="N130" s="1"/>
       <c r="O130" s="1"/>
@@ -4392,7 +4388,7 @@
       <c r="AJ130" s="1"/>
       <c r="AK130" s="1"/>
     </row>
-    <row r="131" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="131" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M131" s="1"/>
       <c r="N131" s="1"/>
       <c r="O131" s="1"/>
@@ -4419,7 +4415,7 @@
       <c r="AJ131" s="1"/>
       <c r="AK131" s="1"/>
     </row>
-    <row r="132" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="132" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M132" s="1"/>
       <c r="N132" s="1"/>
       <c r="O132" s="1"/>
@@ -4446,7 +4442,7 @@
       <c r="AJ132" s="1"/>
       <c r="AK132" s="1"/>
     </row>
-    <row r="133" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="133" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M133" s="1"/>
       <c r="N133" s="1"/>
       <c r="O133" s="1"/>
@@ -4473,7 +4469,7 @@
       <c r="AJ133" s="1"/>
       <c r="AK133" s="1"/>
     </row>
-    <row r="134" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="134" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M134" s="1"/>
       <c r="N134" s="1"/>
       <c r="O134" s="1"/>
@@ -4500,7 +4496,7 @@
       <c r="AJ134" s="1"/>
       <c r="AK134" s="1"/>
     </row>
-    <row r="135" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="135" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M135" s="1"/>
       <c r="N135" s="1"/>
       <c r="O135" s="1"/>
@@ -4527,7 +4523,7 @@
       <c r="AJ135" s="1"/>
       <c r="AK135" s="1"/>
     </row>
-    <row r="136" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="136" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M136" s="1"/>
       <c r="N136" s="1"/>
       <c r="O136" s="1"/>
@@ -4554,7 +4550,7 @@
       <c r="AJ136" s="1"/>
       <c r="AK136" s="1"/>
     </row>
-    <row r="137" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="137" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M137" s="1"/>
       <c r="N137" s="1"/>
       <c r="O137" s="1"/>
@@ -4581,7 +4577,7 @@
       <c r="AJ137" s="1"/>
       <c r="AK137" s="1"/>
     </row>
-    <row r="138" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="138" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M138" s="1"/>
       <c r="N138" s="1"/>
       <c r="O138" s="1"/>
@@ -4608,7 +4604,7 @@
       <c r="AJ138" s="1"/>
       <c r="AK138" s="1"/>
     </row>
-    <row r="139" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="139" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M139" s="1"/>
       <c r="N139" s="1"/>
       <c r="O139" s="1"/>
@@ -4635,7 +4631,7 @@
       <c r="AJ139" s="1"/>
       <c r="AK139" s="1"/>
     </row>
-    <row r="140" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="140" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M140" s="1"/>
       <c r="N140" s="1"/>
       <c r="O140" s="1"/>
@@ -4662,7 +4658,7 @@
       <c r="AJ140" s="1"/>
       <c r="AK140" s="1"/>
     </row>
-    <row r="141" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="141" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M141" s="1"/>
       <c r="N141" s="1"/>
       <c r="O141" s="1"/>
@@ -4689,7 +4685,7 @@
       <c r="AJ141" s="1"/>
       <c r="AK141" s="1"/>
     </row>
-    <row r="142" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="142" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M142" s="1"/>
       <c r="N142" s="1"/>
       <c r="O142" s="1"/>
@@ -4716,7 +4712,7 @@
       <c r="AJ142" s="1"/>
       <c r="AK142" s="1"/>
     </row>
-    <row r="143" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="143" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M143" s="1"/>
       <c r="N143" s="1"/>
       <c r="O143" s="1"/>
@@ -4743,7 +4739,7 @@
       <c r="AJ143" s="1"/>
       <c r="AK143" s="1"/>
     </row>
-    <row r="144" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="144" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M144" s="1"/>
       <c r="N144" s="1"/>
       <c r="O144" s="1"/>
@@ -4770,7 +4766,7 @@
       <c r="AJ144" s="1"/>
       <c r="AK144" s="1"/>
     </row>
-    <row r="145" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="145" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M145" s="1"/>
       <c r="N145" s="1"/>
       <c r="O145" s="1"/>
@@ -4797,7 +4793,7 @@
       <c r="AJ145" s="1"/>
       <c r="AK145" s="1"/>
     </row>
-    <row r="146" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="146" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M146" s="1"/>
       <c r="N146" s="1"/>
       <c r="O146" s="1"/>
@@ -4824,7 +4820,7 @@
       <c r="AJ146" s="1"/>
       <c r="AK146" s="1"/>
     </row>
-    <row r="147" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="147" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M147" s="1"/>
       <c r="N147" s="1"/>
       <c r="O147" s="1"/>
@@ -4851,7 +4847,7 @@
       <c r="AJ147" s="1"/>
       <c r="AK147" s="1"/>
     </row>
-    <row r="148" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="148" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M148" s="1"/>
       <c r="N148" s="1"/>
       <c r="O148" s="1"/>
@@ -4878,7 +4874,7 @@
       <c r="AJ148" s="1"/>
       <c r="AK148" s="1"/>
     </row>
-    <row r="149" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="149" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M149" s="1"/>
       <c r="N149" s="1"/>
       <c r="O149" s="1"/>
@@ -4905,7 +4901,7 @@
       <c r="AJ149" s="1"/>
       <c r="AK149" s="1"/>
     </row>
-    <row r="150" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="150" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M150" s="1"/>
       <c r="N150" s="1"/>
       <c r="O150" s="1"/>
@@ -4932,7 +4928,7 @@
       <c r="AJ150" s="1"/>
       <c r="AK150" s="1"/>
     </row>
-    <row r="151" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="151" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M151" s="1"/>
       <c r="N151" s="1"/>
       <c r="O151" s="1"/>
@@ -4959,7 +4955,7 @@
       <c r="AJ151" s="1"/>
       <c r="AK151" s="1"/>
     </row>
-    <row r="152" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="152" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M152" s="1"/>
       <c r="N152" s="1"/>
       <c r="O152" s="1"/>
@@ -4986,7 +4982,7 @@
       <c r="AJ152" s="1"/>
       <c r="AK152" s="1"/>
     </row>
-    <row r="153" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="153" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M153" s="1"/>
       <c r="N153" s="1"/>
       <c r="O153" s="1"/>
@@ -5013,7 +5009,7 @@
       <c r="AJ153" s="1"/>
       <c r="AK153" s="1"/>
     </row>
-    <row r="154" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="154" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M154" s="1"/>
       <c r="N154" s="1"/>
       <c r="O154" s="1"/>
@@ -5040,7 +5036,7 @@
       <c r="AJ154" s="1"/>
       <c r="AK154" s="1"/>
     </row>
-    <row r="155" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="155" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M155" s="1"/>
       <c r="N155" s="1"/>
       <c r="O155" s="1"/>
@@ -5067,7 +5063,7 @@
       <c r="AJ155" s="1"/>
       <c r="AK155" s="1"/>
     </row>
-    <row r="156" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="156" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M156" s="1"/>
       <c r="N156" s="1"/>
       <c r="O156" s="1"/>
@@ -5094,7 +5090,7 @@
       <c r="AJ156" s="1"/>
       <c r="AK156" s="1"/>
     </row>
-    <row r="157" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="157" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M157" s="1"/>
       <c r="N157" s="1"/>
       <c r="O157" s="1"/>
@@ -5121,7 +5117,7 @@
       <c r="AJ157" s="1"/>
       <c r="AK157" s="1"/>
     </row>
-    <row r="158" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="158" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M158" s="1"/>
       <c r="N158" s="1"/>
       <c r="O158" s="1"/>
@@ -5148,7 +5144,7 @@
       <c r="AJ158" s="1"/>
       <c r="AK158" s="1"/>
     </row>
-    <row r="159" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="159" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M159" s="1"/>
       <c r="N159" s="1"/>
       <c r="O159" s="1"/>
@@ -5175,7 +5171,7 @@
       <c r="AJ159" s="1"/>
       <c r="AK159" s="1"/>
     </row>
-    <row r="160" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="160" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M160" s="1"/>
       <c r="N160" s="1"/>
       <c r="O160" s="1"/>
@@ -5202,7 +5198,7 @@
       <c r="AJ160" s="1"/>
       <c r="AK160" s="1"/>
     </row>
-    <row r="161" spans="13:37" x14ac:dyDescent="0.3">
+    <row r="161" spans="13:37" x14ac:dyDescent="0.25">
       <c r="M161" s="1"/>
       <c r="N161" s="1"/>
       <c r="O161" s="1"/>
@@ -5231,16 +5227,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D11:F14"/>
-    <mergeCell ref="G11:I14"/>
-    <mergeCell ref="J11:L14"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="A3:C6"/>
-    <mergeCell ref="D3:F6"/>
-    <mergeCell ref="G3:I6"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="M3:O6"/>
     <mergeCell ref="M7:O10"/>
@@ -5257,6 +5243,16 @@
     <mergeCell ref="G7:I10"/>
     <mergeCell ref="J7:L10"/>
     <mergeCell ref="A11:C14"/>
+    <mergeCell ref="D11:F14"/>
+    <mergeCell ref="G11:I14"/>
+    <mergeCell ref="J11:L14"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="A3:C6"/>
+    <mergeCell ref="D3:F6"/>
+    <mergeCell ref="G3:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5264,21 +5260,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008EA8F6205B617B4CBD762DBD6D300502" ma:contentTypeVersion="4" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="000a41c94a85e4495c2f2d3453c30ed1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="10b95d85-a823-4616-89f6-0a6587d88b0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0729d4038857d2ede91d1e28869f4e90" ns3:_="">
     <xsd:import namespace="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
@@ -5424,31 +5405,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A7B2E4-0806-468A-9362-8AC839DA2BE7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A39B317-7C09-4361-8F9C-EC6B55EB4D12}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5464,4 +5436,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A7B2E4-0806-468A-9362-8AC839DA2BE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
member1: update no backlog e review do use case
</commit_message>
<xml_diff>
--- a/scrum/Phase1/Sprint1/Sprint_backlog.xlsx
+++ b/scrum/Phase1/Sprint1/Sprint_backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nova pasta\SE2122_57464_58763_57677_58125_63764\scrum\Phase1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A2FEFB-194E-47F9-BEE5-A22C9A66720A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B7D77C-1223-4693-9A3B-284C94DA9449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{890A83B6-DAA2-4C76-8505-33013FC76E3A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -73,12 +73,6 @@
 Member 4: finished code smells</t>
   </si>
   <si>
-    <t>Member 1: finished Reviews.
-Member 5: finished Reviews.
-Member 2: finished Reviews.
-Member 4: finished Reviews.</t>
-  </si>
-  <si>
     <t>Member 4: Detect 3 code smells in preferences package and review 3 others</t>
   </si>
   <si>
@@ -89,16 +83,6 @@
 Member 5: finished pattern detection
 Member 3: finished pattern detection
 Member 1: finished pattern detection Member 4: finished pattern detection</t>
-  </si>
-  <si>
-    <t>Member 3: model package
-Member 4: do the MOOD metrics set, analyse the result and make a report.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Member 5: finished Reviews.
-Member 1: finished Reviews.
-Member 2: finished Reviews. Member 4: finished Reviews.
-</t>
   </si>
   <si>
     <t xml:space="preserve">Member 5: finished doing the metrics
@@ -113,21 +97,41 @@
 Member 4: preferences package</t>
   </si>
   <si>
-    <t>Member 5: finished Reviews.
-Member 2: finished Reviews. Member 4: finished Reviews.
-Member 1: finished Reviews.</t>
-  </si>
-  <si>
-    <t>Member 4: making diagrams</t>
-  </si>
-  <si>
     <t>Member 5: finished Use case diagrams
+Member 4: finished Use case diagrams
 Member 2: finished Use case diagrams
 Member 1: finished Use case diagrams
 Member 3: making diagrams</t>
   </si>
   <si>
-    <t>Member 3: Reviewing.</t>
+    <t>Member 5: finished Reviews.
+Member 2: finished Reviews. Member 4: finished Reviews.
+Member 1: finished Reviews.
+Member 3: finished Reviews.</t>
+  </si>
+  <si>
+    <t>Member 1: finished Reviews.
+Member 5: finished Reviews.
+Member 2: finished Reviews.
+Member 4: finished Reviews.
+Member 3: finished Reviews.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Member 5: finished Reviews.
+Member 1: finished Reviews.
+Member 2: finished Reviews. Member 4: finished Reviews.
+Member 3: finished Reviews.
+</t>
+  </si>
+  <si>
+    <t>Nothing</t>
+  </si>
+  <si>
+    <t>Member 3: Dependy metrics
+Member 4: MOOD metrics
+Member 1: Complexity metrics
+Member 2:  Lines of Code metrics
+Member 5: Martin package metrics</t>
   </si>
 </sst>
 </file>
@@ -250,17 +254,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -268,14 +269,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -284,6 +282,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -605,7 +609,7 @@
   <dimension ref="A1:AL161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+      <selection activeCell="D15" sqref="D15:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,23 +620,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -658,31 +662,31 @@
       <c r="AL1" s="1"/>
     </row>
     <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="7" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="7" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="7" t="s">
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -707,26 +711,28 @@
       <c r="AK2" s="1"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8" t="s">
+        <v>11</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="12" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="6" t="s">
-        <v>11</v>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -754,18 +760,18 @@
       <c r="AK3" s="1"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -793,18 +799,18 @@
       <c r="AK4" s="1"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
@@ -832,18 +838,18 @@
       <c r="AK5" s="1"/>
     </row>
     <row r="6" spans="1:38" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
@@ -871,27 +877,29 @@
       <c r="AK6" s="1"/>
     </row>
     <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3" t="s">
-        <v>18</v>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="8" t="s">
+        <v>15</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="6" t="s">
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="6" t="s">
-        <v>21</v>
+      <c r="J7" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
+      <c r="M7" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="1"/>
@@ -918,9 +926,9 @@
       <c r="AK7" s="1"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -957,9 +965,9 @@
       <c r="AK8" s="1"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -996,9 +1004,9 @@
       <c r="AK9" s="1"/>
     </row>
     <row r="10" spans="1:38" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -1040,21 +1048,23 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="3" t="s">
-        <v>13</v>
+      <c r="D11" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="6"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="6" t="s">
-        <v>14</v>
+      <c r="J11" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="6" t="s">
-        <v>16</v>
+      <c r="M11" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -1204,23 +1214,23 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="3" t="s">
-        <v>15</v>
+      <c r="D15" s="8" t="s">
+        <v>21</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="6" t="s">
-        <v>22</v>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="6" t="s">
-        <v>17</v>
+      <c r="J15" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
-      <c r="M15" s="6" t="s">
-        <v>19</v>
+      <c r="M15" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
@@ -5227,6 +5237,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D11:F14"/>
+    <mergeCell ref="G11:I14"/>
+    <mergeCell ref="J11:L14"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="A3:C6"/>
+    <mergeCell ref="D3:F6"/>
+    <mergeCell ref="G3:I6"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="M3:O6"/>
     <mergeCell ref="M7:O10"/>
@@ -5243,16 +5263,6 @@
     <mergeCell ref="G7:I10"/>
     <mergeCell ref="J7:L10"/>
     <mergeCell ref="A11:C14"/>
-    <mergeCell ref="D11:F14"/>
-    <mergeCell ref="G11:I14"/>
-    <mergeCell ref="J11:L14"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="A3:C6"/>
-    <mergeCell ref="D3:F6"/>
-    <mergeCell ref="G3:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5260,6 +5270,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008EA8F6205B617B4CBD762DBD6D300502" ma:contentTypeVersion="4" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="000a41c94a85e4495c2f2d3453c30ed1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="10b95d85-a823-4616-89f6-0a6587d88b0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0729d4038857d2ede91d1e28869f4e90" ns3:_="">
     <xsd:import namespace="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
@@ -5405,22 +5430,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A7B2E4-0806-468A-9362-8AC839DA2BE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A39B317-7C09-4361-8F9C-EC6B55EB4D12}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5436,28 +5470,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ADCA16D-8B36-4E58-B5D4-3D3019E41DFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A7B2E4-0806-468A-9362-8AC839DA2BE7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="10b95d85-a823-4616-89f6-0a6587d88b0c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>